<commit_message>
adding pwm to fast api
</commit_message>
<xml_diff>
--- a/documentation/Tabla_de_registros_HMI_Ivan.xlsx
+++ b/documentation/Tabla_de_registros_HMI_Ivan.xlsx
@@ -8,8 +8,8 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Registros para logica" sheetId="1" state="visible" r:id="rId3"/>
-    <sheet name="Registros" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="Registros para logica" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Registros" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Registros!$A$1:$J$1</definedName>
@@ -26,7 +26,7 @@
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author>Unknown Author</author>
+    <author> </author>
   </authors>
   <commentList>
     <comment ref="B131" authorId="0">
@@ -280,7 +280,7 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
         <charset val="1"/>
@@ -291,7 +291,7 @@
       <rPr>
         <b val="true"/>
         <sz val="12"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
         <charset val="1"/>
@@ -301,7 +301,7 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
         <charset val="1"/>
@@ -316,7 +316,7 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
         <charset val="1"/>
@@ -327,7 +327,7 @@
       <rPr>
         <b val="true"/>
         <sz val="12"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
         <charset val="1"/>
@@ -337,7 +337,7 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
         <charset val="1"/>
@@ -352,7 +352,7 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
         <charset val="1"/>
@@ -363,7 +363,7 @@
       <rPr>
         <b val="true"/>
         <sz val="12"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
         <charset val="1"/>
@@ -373,7 +373,7 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
         <charset val="1"/>
@@ -388,7 +388,7 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
         <charset val="1"/>
@@ -399,7 +399,7 @@
       <rPr>
         <b val="true"/>
         <sz val="12"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
         <charset val="1"/>
@@ -409,7 +409,7 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
         <charset val="1"/>
@@ -424,7 +424,7 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
         <charset val="1"/>
@@ -435,7 +435,7 @@
       <rPr>
         <b val="true"/>
         <sz val="12"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
         <charset val="1"/>
@@ -445,7 +445,7 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
         <charset val="1"/>
@@ -853,25 +853,7 @@
     <t xml:space="preserve">Pantalla cambio de cubeta en modo manual</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Entrar Pantalla 0:0 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> (21)</t>
-    </r>
+    <t xml:space="preserve">Entrar Pantalla 0:0  (21)</t>
   </si>
   <si>
     <t xml:space="preserve">CB-0015</t>
@@ -1243,145 +1225,37 @@
     <t xml:space="preserve">sensor_material_pressure </t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">HR-0030 – </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">HR-40048</t>
-    </r>
+    <t xml:space="preserve">HR-0030 – HR-40048</t>
   </si>
   <si>
     <t xml:space="preserve">sensor_material_temperature </t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">HR-0031 – </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">HR-40049</t>
-    </r>
+    <t xml:space="preserve">HR-0031 – HR-40049</t>
   </si>
   <si>
     <t xml:space="preserve">sensor_laser_distance </t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">HR-0032 -</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">HR-40050</t>
-    </r>
+    <t xml:space="preserve">HR-0032 -HR-40050</t>
   </si>
   <si>
     <t xml:space="preserve">sensor_pressure_regulator_read_set </t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">HR-0033 – </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">HR-40051</t>
-    </r>
+    <t xml:space="preserve">HR-0033 – HR-40051</t>
   </si>
   <si>
     <t xml:space="preserve">sensor_pressure_regulator_read_real </t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">HR-0034 – </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">HR-40052</t>
-    </r>
+    <t xml:space="preserve">HR-0034 – HR-40052</t>
   </si>
   <si>
     <t xml:space="preserve">sensor_pressure_regulator_valve_read_state </t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">HR-0035 – </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">HR-40053</t>
-    </r>
+    <t xml:space="preserve">HR-0035 – HR-40053</t>
   </si>
   <si>
     <t xml:space="preserve">Datos</t>
@@ -1461,10 +1335,10 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="_-\$* #,##0.00_-;&quot;-$&quot;* #,##0.00_-;_-\$* \-??_-;_-@_-"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="12">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -1486,7 +1360,7 @@
     </font>
     <font>
       <sz val="12"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="1"/>
@@ -1494,7 +1368,7 @@
     <font>
       <b val="true"/>
       <sz val="12"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="1"/>
@@ -1502,6 +1376,14 @@
     <font>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="1"/>
@@ -1517,26 +1399,13 @@
     <font>
       <b val="true"/>
       <sz val="16"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="1"/>
     </font>
     <font>
-      <sz val="12"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
@@ -1549,12 +1418,18 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FF003300"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -1564,19 +1439,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor rgb="FF70AD47"/>
         <bgColor rgb="FF339966"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor rgb="FFFFC000"/>
         <bgColor rgb="FFFF9900"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFF5CE"/>
       </patternFill>
     </fill>
@@ -1852,27 +1727,27 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1964,16 +1839,88 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -2008,87 +1955,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="6" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2104,11 +1979,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2132,11 +2007,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="6" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2152,15 +2027,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="6" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="6" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="6" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2172,15 +2047,15 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="6" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="10" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2188,11 +2063,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2275,23 +2150,6 @@
     <cellStyle name="Moneda 2" xfId="20"/>
     <cellStyle name="Moneda 3" xfId="21"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF000000"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -2359,180 +2217,8 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Tema de Office">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:srgbClr val="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:srgbClr val="ffffff"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="44546a"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="e7e6e6"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="5b9bd5"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="ed7d31"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="a5a5a5"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="ffc000"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="4472c4"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="70ad47"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0563c1"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="954f72"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204" pitchFamily="0" charset="1"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="0" charset="1"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme>
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:tint val="73000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:tint val="81000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
-        </a:gradFill>
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:shade val="78000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -2542,7 +2228,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.57"/>
@@ -2551,8 +2237,8 @@
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2561,29 +2247,29 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:L308"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A118" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B137" activeCellId="0" sqref="B137"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.4453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="26.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="61.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="45.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="34.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="18.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="13.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="20.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="24.14"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="11" style="1" width="11.43"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="11" style="1" width="11.43"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7632,8 +7318,8 @@
     <mergeCell ref="A145:A149"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
control logic with hamilton
</commit_message>
<xml_diff>
--- a/documentation/Tabla_de_registros_HMI_Ivan.xlsx
+++ b/documentation/Tabla_de_registros_HMI_Ivan.xlsx
@@ -8,8 +8,8 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Registros para logica" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Registros" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Registros para logica" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Registros" sheetId="2" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Registros!$A$1:$J$1</definedName>
@@ -26,7 +26,7 @@
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author> </author>
+    <author>Unknown Author</author>
   </authors>
   <commentList>
     <comment ref="B131" authorId="0">
@@ -36,7 +36,6 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">These goes to the HMI, will add the sensor reading to be displayed here, which are the values from IOLink data</t>
         </r>
@@ -103,7 +102,7 @@
     <t xml:space="preserve">MW101</t>
   </si>
   <si>
-    <t xml:space="preserve">Sensor de distancia </t>
+    <t xml:space="preserve">Sensor de distancia (laser)</t>
   </si>
   <si>
     <t xml:space="preserve">Lectura de distancia</t>
@@ -280,10 +279,9 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <color rgb="FF000000"/>
+        <color theme="1"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Cubeta llena entre el 100 y 80 </t>
     </r>
@@ -294,7 +292,6 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(Lleno</t>
     </r>
@@ -304,7 +301,6 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">)</t>
     </r>
@@ -316,10 +312,9 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <color rgb="FF000000"/>
+        <color theme="1"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Cubeta entre el 79 y 50 (</t>
     </r>
@@ -330,7 +325,6 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Medio-alto</t>
     </r>
@@ -340,7 +334,6 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">)</t>
     </r>
@@ -352,10 +345,9 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <color rgb="FF000000"/>
+        <color theme="1"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Cubeta entre el 49 y 30 (</t>
     </r>
@@ -366,7 +358,6 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Medio</t>
     </r>
@@ -376,7 +367,6 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">)</t>
     </r>
@@ -388,10 +378,9 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <color rgb="FF000000"/>
+        <color theme="1"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Cubeta entre el 20 y 10 (</t>
     </r>
@@ -402,7 +391,6 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Prevacio</t>
     </r>
@@ -412,7 +400,6 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">)</t>
     </r>
@@ -424,10 +411,9 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <color rgb="FF000000"/>
+        <color theme="1"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Cubeta entre el 5 hacia abajo (2cm) (</t>
     </r>
@@ -438,7 +424,6 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Vacio</t>
     </r>
@@ -448,7 +433,6 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">)</t>
     </r>
@@ -1225,37 +1209,139 @@
     <t xml:space="preserve">sensor_material_pressure </t>
   </si>
   <si>
-    <t xml:space="preserve">HR-0030 – HR-40048</t>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">HR-0030 – </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">HR-40048</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">sensor_material_temperature </t>
   </si>
   <si>
-    <t xml:space="preserve">HR-0031 – HR-40049</t>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">HR-0031 – </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">HR-40049</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">sensor_laser_distance </t>
   </si>
   <si>
-    <t xml:space="preserve">HR-0032 -HR-40050</t>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">HR-0032 -</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">HR-40050</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">sensor_pressure_regulator_read_set </t>
   </si>
   <si>
-    <t xml:space="preserve">HR-0033 – HR-40051</t>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">HR-0033 – </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">HR-40051</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">sensor_pressure_regulator_read_real </t>
   </si>
   <si>
-    <t xml:space="preserve">HR-0034 – HR-40052</t>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">HR-0034 – </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">HR-40052</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">sensor_pressure_regulator_valve_read_state </t>
   </si>
   <si>
-    <t xml:space="preserve">HR-0035 – HR-40053</t>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">HR-0035 – </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">HR-40053</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Datos</t>
@@ -1335,13 +1421,12 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="_-\$* #,##0.00_-;&quot;-$&quot;* #,##0.00_-;_-\$* \-??_-;_-@_-"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1360,25 +1445,22 @@
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="12"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -1386,50 +1468,45 @@
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
-      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <u val="single"/>
       <sz val="24"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="16"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF000000"/>
-        <bgColor rgb="FF003300"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -1439,19 +1516,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF70AD47"/>
+        <fgColor theme="9"/>
         <bgColor rgb="FF339966"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
+        <fgColor theme="7"/>
         <bgColor rgb="FFFF9900"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
+        <fgColor theme="0"/>
         <bgColor rgb="FFFFF5CE"/>
       </patternFill>
     </fill>
@@ -1718,7 +1795,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="105">
+  <cellXfs count="106">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1727,27 +1804,27 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1839,16 +1916,52 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1887,20 +2000,36 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1911,59 +2040,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="6" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1979,11 +2056,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2007,11 +2084,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="7" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="6" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2027,15 +2104,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="7" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="6" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="7" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="6" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="7" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="6" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2047,15 +2128,15 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="7" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="6" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="11" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2063,11 +2144,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2150,6 +2231,23 @@
     <cellStyle name="Moneda 2" xfId="20"/>
     <cellStyle name="Moneda 3" xfId="21"/>
   </cellStyles>
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -2217,8 +2315,114 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Tema de Office">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546a"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="e7e6e6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5b9bd5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ed7d31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a5a5a5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="ffc000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472c4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70ad47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563c1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954f72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -2228,17 +2432,19 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="24"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+  </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2247,29 +2453,29 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:L308"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.4453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="26.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="61.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="45.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="34.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="18.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="13.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="20.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="24.14"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="11" style="1" width="11.43"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="11" style="1" width="11.43"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2330,7 +2536,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="8"/>
       <c r="B3" s="14" t="s">
         <v>16</v>
@@ -2412,7 +2618,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="8"/>
       <c r="B6" s="24" t="s">
         <v>26</v>
@@ -2544,7 +2750,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="8" t="s">
         <v>47</v>
       </c>
@@ -2646,7 +2852,7 @@
       <c r="I14" s="12"/>
       <c r="J14" s="29"/>
     </row>
-    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="8"/>
       <c r="B15" s="30" t="s">
         <v>60</v>
@@ -2718,7 +2924,7 @@
       <c r="I17" s="12"/>
       <c r="J17" s="29"/>
     </row>
-    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="8"/>
       <c r="B18" s="23" t="s">
         <v>68</v>
@@ -2742,7 +2948,7 @@
       <c r="I18" s="12"/>
       <c r="J18" s="29"/>
     </row>
-    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="8"/>
       <c r="B19" s="23" t="s">
         <v>71</v>
@@ -2796,7 +3002,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="8"/>
       <c r="B21" s="33"/>
       <c r="C21" s="37" t="n">
@@ -2820,7 +3026,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="8"/>
       <c r="B22" s="33"/>
       <c r="C22" s="37" t="n">
@@ -2844,7 +3050,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="8"/>
       <c r="B23" s="33"/>
       <c r="C23" s="37" t="n">
@@ -2868,7 +3074,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="8"/>
       <c r="B24" s="33"/>
       <c r="C24" s="37" t="n">
@@ -2892,7 +3098,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="8"/>
       <c r="B25" s="33"/>
       <c r="C25" s="37" t="n">
@@ -2916,7 +3122,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="8"/>
       <c r="B26" s="33"/>
       <c r="C26" s="37" t="n">
@@ -2940,7 +3146,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="8"/>
       <c r="B27" s="33"/>
       <c r="C27" s="39" t="n">
@@ -2964,7 +3170,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="8"/>
       <c r="B28" s="41" t="s">
         <v>77</v>
@@ -2992,7 +3198,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="8"/>
       <c r="B29" s="41"/>
       <c r="C29" s="37" t="n">
@@ -3016,7 +3222,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="8"/>
       <c r="B30" s="41"/>
       <c r="C30" s="37" t="n">
@@ -3040,7 +3246,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="8"/>
       <c r="B31" s="41"/>
       <c r="C31" s="37" t="n">
@@ -3064,7 +3270,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="8"/>
       <c r="B32" s="41"/>
       <c r="C32" s="37" t="n">
@@ -3088,7 +3294,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="8"/>
       <c r="B33" s="41"/>
       <c r="C33" s="37" t="n">
@@ -3112,7 +3318,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="8"/>
       <c r="B34" s="41"/>
       <c r="C34" s="37" t="n">
@@ -3136,7 +3342,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="8"/>
       <c r="B35" s="41"/>
       <c r="C35" s="37" t="n">
@@ -3188,7 +3394,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="8"/>
       <c r="B37" s="42"/>
       <c r="C37" s="46" t="n">
@@ -3212,7 +3418,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="8"/>
       <c r="B38" s="42"/>
       <c r="C38" s="46" t="n">
@@ -3236,7 +3442,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="8"/>
       <c r="B39" s="42"/>
       <c r="C39" s="46" t="n">
@@ -3260,7 +3466,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="8"/>
       <c r="B40" s="42"/>
       <c r="C40" s="46" t="n">
@@ -3284,7 +3490,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="8"/>
       <c r="B41" s="42"/>
       <c r="C41" s="46" t="n">
@@ -3308,7 +3514,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="8"/>
       <c r="B42" s="42"/>
       <c r="C42" s="46" t="n">
@@ -3332,7 +3538,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="8"/>
       <c r="B43" s="42"/>
       <c r="C43" s="48" t="n">
@@ -3384,7 +3590,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="8"/>
       <c r="B45" s="50"/>
       <c r="C45" s="46" t="n">
@@ -3408,7 +3614,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="8"/>
       <c r="B46" s="50"/>
       <c r="C46" s="46" t="n">
@@ -3432,7 +3638,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="8"/>
       <c r="B47" s="50"/>
       <c r="C47" s="46" t="n">
@@ -3456,7 +3662,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="8"/>
       <c r="B48" s="50"/>
       <c r="C48" s="46" t="n">
@@ -3480,7 +3686,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="8"/>
       <c r="B49" s="50"/>
       <c r="C49" s="46" t="n">
@@ -3504,7 +3710,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="8"/>
       <c r="B50" s="50"/>
       <c r="C50" s="46" t="n">
@@ -3528,7 +3734,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="8"/>
       <c r="B51" s="50"/>
       <c r="C51" s="46" t="n">
@@ -3552,7 +3758,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="8"/>
       <c r="B52" s="51" t="s">
         <v>83</v>
@@ -3580,7 +3786,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="8"/>
       <c r="B53" s="51"/>
       <c r="C53" s="55" t="n">
@@ -3604,7 +3810,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="8"/>
       <c r="B54" s="51"/>
       <c r="C54" s="55" t="n">
@@ -3628,7 +3834,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="8"/>
       <c r="B55" s="51"/>
       <c r="C55" s="55" t="n">
@@ -3652,7 +3858,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="8"/>
       <c r="B56" s="51"/>
       <c r="C56" s="55" t="n">
@@ -3676,7 +3882,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="8"/>
       <c r="B57" s="51"/>
       <c r="C57" s="55" t="n">
@@ -3700,7 +3906,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="8"/>
       <c r="B58" s="51"/>
       <c r="C58" s="55" t="n">
@@ -3724,7 +3930,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="8"/>
       <c r="B59" s="51"/>
       <c r="C59" s="57" t="n">
@@ -3776,7 +3982,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="8"/>
       <c r="B61" s="27"/>
       <c r="C61" s="59" t="n">
@@ -3800,7 +4006,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="8"/>
       <c r="B62" s="27"/>
       <c r="C62" s="59" t="n">
@@ -3824,7 +4030,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="8"/>
       <c r="B63" s="27"/>
       <c r="C63" s="59" t="n">
@@ -3848,7 +4054,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="8"/>
       <c r="B64" s="27"/>
       <c r="C64" s="59" t="n">
@@ -3872,7 +4078,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="8"/>
       <c r="B65" s="27"/>
       <c r="C65" s="59" t="n">
@@ -3896,7 +4102,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="8"/>
       <c r="B66" s="27"/>
       <c r="C66" s="59" t="n">
@@ -3920,7 +4126,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="8"/>
       <c r="B67" s="27"/>
       <c r="C67" s="59" t="n">
@@ -4000,7 +4206,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E70" s="64"/>
     </row>
     <row r="71" customFormat="false" ht="56.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4015,6 +4221,7 @@
         <v>98</v>
       </c>
     </row>
+    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="73" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="66" t="s">
         <v>99</v>
@@ -4096,7 +4303,7 @@
       <c r="I76" s="71"/>
       <c r="J76" s="71"/>
     </row>
-    <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="72" t="s">
         <v>114</v>
       </c>
@@ -4168,7 +4375,7 @@
       </c>
       <c r="F80" s="64"/>
     </row>
-    <row r="81" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="23" t="s">
         <v>130</v>
       </c>
@@ -4222,7 +4429,7 @@
       </c>
       <c r="F83" s="64"/>
     </row>
-    <row r="84" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="23" t="s">
         <v>143</v>
       </c>
@@ -4243,7 +4450,7 @@
       <c r="H84" s="64"/>
       <c r="I84" s="64"/>
     </row>
-    <row r="85" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="23" t="s">
         <v>147</v>
       </c>
@@ -4264,7 +4471,7 @@
       <c r="H85" s="64"/>
       <c r="I85" s="64"/>
     </row>
-    <row r="86" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A86" s="23" t="s">
         <v>151</v>
       </c>
@@ -4288,7 +4495,7 @@
       <c r="I86" s="71"/>
       <c r="J86" s="71"/>
     </row>
-    <row r="87" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="23" t="s">
         <v>156</v>
       </c>
@@ -4308,7 +4515,7 @@
       <c r="G87" s="64"/>
       <c r="I87" s="64"/>
     </row>
-    <row r="88" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="72" t="s">
         <v>160</v>
       </c>
@@ -4377,7 +4584,7 @@
       <c r="I90" s="71"/>
       <c r="J90" s="71"/>
     </row>
-    <row r="91" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="72" t="s">
         <v>175</v>
       </c>
@@ -4482,7 +4689,7 @@
       <c r="H95" s="64"/>
       <c r="I95" s="64"/>
     </row>
-    <row r="96" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="23" t="s">
         <v>195</v>
       </c>
@@ -4503,7 +4710,7 @@
       <c r="H96" s="64"/>
       <c r="I96" s="64"/>
     </row>
-    <row r="97" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="23" t="s">
         <v>199</v>
       </c>
@@ -4524,7 +4731,7 @@
       <c r="H97" s="64"/>
       <c r="I97" s="64"/>
     </row>
-    <row r="98" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="23" t="s">
         <v>203</v>
       </c>
@@ -4545,7 +4752,7 @@
       <c r="H98" s="64"/>
       <c r="I98" s="64"/>
     </row>
-    <row r="99" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="23" t="s">
         <v>207</v>
       </c>
@@ -4590,7 +4797,7 @@
       <c r="I100" s="71"/>
       <c r="J100" s="71"/>
     </row>
-    <row r="101" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="23" t="s">
         <v>130</v>
       </c>
@@ -4611,8 +4818,8 @@
       <c r="H101" s="64"/>
       <c r="I101" s="64"/>
     </row>
-    <row r="102" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="23" t="s">
+    <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="79" t="s">
         <v>218</v>
       </c>
       <c r="B102" s="67" t="s">
@@ -4653,7 +4860,7 @@
       <c r="H103" s="64"/>
       <c r="I103" s="64"/>
     </row>
-    <row r="104" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="23" t="s">
         <v>227</v>
       </c>
@@ -4696,7 +4903,7 @@
       <c r="I105" s="64"/>
     </row>
     <row r="106" customFormat="false" ht="74.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A106" s="79" t="s">
+      <c r="A106" s="80" t="s">
         <v>233</v>
       </c>
       <c r="B106" s="73" t="s">
@@ -4736,7 +4943,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="108" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="72" t="s">
         <v>243</v>
       </c>
@@ -4753,7 +4960,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="109" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="72" t="s">
         <v>247</v>
       </c>
@@ -4771,7 +4978,7 @@
       </c>
     </row>
     <row r="110" customFormat="false" ht="142.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A110" s="80" t="s">
+      <c r="A110" s="81" t="s">
         <v>251</v>
       </c>
       <c r="B110" s="67" t="s">
@@ -4795,7 +5002,7 @@
       <c r="J110" s="8"/>
     </row>
     <row r="111" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A111" s="80" t="s">
+      <c r="A111" s="81" t="s">
         <v>257</v>
       </c>
       <c r="B111" s="67" t="s">
@@ -4815,7 +5022,7 @@
       <c r="H111" s="64"/>
       <c r="I111" s="64"/>
     </row>
-    <row r="112" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="112" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A112" s="23" t="s">
         <v>261</v>
       </c>
@@ -4838,7 +5045,7 @@
       <c r="H112" s="8"/>
       <c r="I112" s="8"/>
     </row>
-    <row r="113" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="23" t="s">
         <v>265</v>
       </c>
@@ -4859,7 +5066,7 @@
       <c r="I113" s="64"/>
     </row>
     <row r="114" customFormat="false" ht="26.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A114" s="80" t="s">
+      <c r="A114" s="81" t="s">
         <v>268</v>
       </c>
       <c r="B114" s="67" t="s">
@@ -4874,13 +5081,13 @@
       <c r="E114" s="70" t="s">
         <v>255</v>
       </c>
-      <c r="F114" s="81" t="s">
+      <c r="F114" s="82" t="s">
         <v>272</v>
       </c>
-      <c r="G114" s="81"/>
-      <c r="H114" s="81"/>
-      <c r="I114" s="81"/>
-      <c r="J114" s="81"/>
+      <c r="G114" s="82"/>
+      <c r="H114" s="82"/>
+      <c r="I114" s="82"/>
+      <c r="J114" s="82"/>
     </row>
     <row r="115" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A115" s="23" t="s">
@@ -4903,7 +5110,7 @@
       <c r="H115" s="64"/>
       <c r="I115" s="64"/>
     </row>
-    <row r="116" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="72" t="s">
         <v>276</v>
       </c>
@@ -4924,7 +5131,7 @@
       <c r="H116" s="64"/>
       <c r="I116" s="64"/>
     </row>
-    <row r="117" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="72" t="s">
         <v>281</v>
       </c>
@@ -4945,7 +5152,7 @@
       <c r="H117" s="64"/>
       <c r="I117" s="64"/>
     </row>
-    <row r="118" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="72" t="s">
         <v>285</v>
       </c>
@@ -4966,7 +5173,7 @@
       <c r="H118" s="64"/>
       <c r="I118" s="64"/>
     </row>
-    <row r="119" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="72" t="s">
         <v>289</v>
       </c>
@@ -4987,7 +5194,7 @@
       <c r="H119" s="64"/>
       <c r="I119" s="64"/>
     </row>
-    <row r="120" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="72" t="s">
         <v>293</v>
       </c>
@@ -5009,7 +5216,7 @@
       <c r="I120" s="8"/>
       <c r="J120" s="8"/>
     </row>
-    <row r="121" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="72" t="s">
         <v>297</v>
       </c>
@@ -5030,7 +5237,7 @@
       <c r="H121" s="64"/>
       <c r="I121" s="64"/>
     </row>
-    <row r="122" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="72" t="s">
         <v>301</v>
       </c>
@@ -5051,7 +5258,7 @@
       <c r="H122" s="64"/>
       <c r="I122" s="64"/>
     </row>
-    <row r="123" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="23" t="s">
         <v>305</v>
       </c>
@@ -5072,7 +5279,7 @@
       <c r="H123" s="64"/>
       <c r="I123" s="64"/>
     </row>
-    <row r="124" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="23" t="s">
         <v>309</v>
       </c>
@@ -5093,7 +5300,7 @@
       <c r="H124" s="64"/>
       <c r="I124" s="64"/>
     </row>
-    <row r="125" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="23" t="s">
         <v>313</v>
       </c>
@@ -5114,7 +5321,7 @@
       <c r="H125" s="64"/>
       <c r="I125" s="64"/>
     </row>
-    <row r="126" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="72" t="s">
         <v>317</v>
       </c>
@@ -5135,7 +5342,7 @@
       <c r="H126" s="64"/>
       <c r="I126" s="64"/>
     </row>
-    <row r="127" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="72" t="s">
         <v>322</v>
       </c>
@@ -5156,7 +5363,7 @@
       <c r="H127" s="64"/>
       <c r="I127" s="64"/>
     </row>
-    <row r="128" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="72" t="s">
         <v>326</v>
       </c>
@@ -5178,7 +5385,7 @@
       <c r="I128" s="64"/>
     </row>
     <row r="129" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A129" s="82" t="s">
+      <c r="A129" s="83" t="s">
         <v>330</v>
       </c>
       <c r="B129" s="73" t="s">
@@ -5198,7 +5405,7 @@
       <c r="H129" s="64"/>
       <c r="I129" s="64"/>
     </row>
-    <row r="130" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="72" t="s">
         <v>334</v>
       </c>
@@ -5219,11 +5426,11 @@
       <c r="H130" s="64"/>
       <c r="I130" s="64"/>
     </row>
-    <row r="131" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A131" s="83" t="s">
+    <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A131" s="84" t="s">
         <v>338</v>
       </c>
-      <c r="B131" s="84" t="s">
+      <c r="B131" s="85" t="s">
         <v>339</v>
       </c>
       <c r="C131" s="64"/>
@@ -5234,11 +5441,11 @@
       <c r="H131" s="64"/>
       <c r="I131" s="64"/>
     </row>
-    <row r="132" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A132" s="83" t="s">
+    <row r="132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A132" s="84" t="s">
         <v>340</v>
       </c>
-      <c r="B132" s="84" t="s">
+      <c r="B132" s="85" t="s">
         <v>341</v>
       </c>
       <c r="C132" s="64"/>
@@ -5249,11 +5456,11 @@
       <c r="H132" s="64"/>
       <c r="I132" s="64"/>
     </row>
-    <row r="133" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A133" s="83" t="s">
+    <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A133" s="84" t="s">
         <v>342</v>
       </c>
-      <c r="B133" s="84" t="s">
+      <c r="B133" s="85" t="s">
         <v>343</v>
       </c>
       <c r="C133" s="64"/>
@@ -5264,11 +5471,11 @@
       <c r="H133" s="64"/>
       <c r="I133" s="64"/>
     </row>
-    <row r="134" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A134" s="83" t="s">
+    <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A134" s="84" t="s">
         <v>344</v>
       </c>
-      <c r="B134" s="84" t="s">
+      <c r="B134" s="85" t="s">
         <v>345</v>
       </c>
       <c r="C134" s="64"/>
@@ -5279,11 +5486,11 @@
       <c r="H134" s="64"/>
       <c r="I134" s="64"/>
     </row>
-    <row r="135" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A135" s="83" t="s">
+    <row r="135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A135" s="84" t="s">
         <v>346</v>
       </c>
-      <c r="B135" s="84" t="s">
+      <c r="B135" s="85" t="s">
         <v>347</v>
       </c>
       <c r="C135" s="64"/>
@@ -5294,11 +5501,11 @@
       <c r="H135" s="64"/>
       <c r="I135" s="64"/>
     </row>
-    <row r="136" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A136" s="83" t="s">
+    <row r="136" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A136" s="84" t="s">
         <v>348</v>
       </c>
-      <c r="B136" s="84" t="s">
+      <c r="B136" s="85" t="s">
         <v>349</v>
       </c>
       <c r="C136" s="64"/>
@@ -5309,7 +5516,7 @@
       <c r="H136" s="64"/>
       <c r="I136" s="64"/>
     </row>
-    <row r="137" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="137" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B137" s="64"/>
       <c r="C137" s="64"/>
       <c r="D137" s="64"/>
@@ -5319,7 +5526,7 @@
       <c r="H137" s="64"/>
       <c r="I137" s="64"/>
     </row>
-    <row r="138" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="138" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B138" s="64"/>
       <c r="C138" s="64"/>
       <c r="D138" s="64"/>
@@ -5329,7 +5536,7 @@
       <c r="H138" s="64"/>
       <c r="I138" s="64"/>
     </row>
-    <row r="139" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="139" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B139" s="64"/>
       <c r="C139" s="64"/>
       <c r="D139" s="64"/>
@@ -5339,7 +5546,7 @@
       <c r="H139" s="64"/>
       <c r="I139" s="64"/>
     </row>
-    <row r="140" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="140" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="64"/>
       <c r="B140" s="64"/>
       <c r="C140" s="64"/>
@@ -5350,7 +5557,7 @@
       <c r="H140" s="64"/>
       <c r="I140" s="64"/>
     </row>
-    <row r="141" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="141" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="64"/>
       <c r="B141" s="64"/>
       <c r="C141" s="64"/>
@@ -5361,7 +5568,7 @@
       <c r="H141" s="64"/>
       <c r="I141" s="64"/>
     </row>
-    <row r="142" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="142" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="64"/>
       <c r="B142" s="64"/>
       <c r="C142" s="64"/>
@@ -5373,14 +5580,14 @@
       <c r="I142" s="64"/>
     </row>
     <row r="143" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A143" s="85"/>
-      <c r="B143" s="86" t="s">
+      <c r="A143" s="86"/>
+      <c r="B143" s="87" t="s">
         <v>350</v>
       </c>
-      <c r="C143" s="86" t="s">
+      <c r="C143" s="87" t="s">
         <v>351</v>
       </c>
-      <c r="D143" s="87" t="s">
+      <c r="D143" s="88" t="s">
         <v>352</v>
       </c>
       <c r="E143" s="67" t="s">
@@ -5393,8 +5600,8 @@
       <c r="H143" s="64"/>
       <c r="I143" s="64"/>
     </row>
-    <row r="144" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A144" s="88"/>
+    <row r="144" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A144" s="89"/>
       <c r="B144" s="64"/>
       <c r="C144" s="64"/>
       <c r="D144" s="64"/>
@@ -5405,16 +5612,16 @@
       <c r="I144" s="64"/>
     </row>
     <row r="145" customFormat="false" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A145" s="89" t="s">
+      <c r="A145" s="90" t="s">
         <v>353</v>
       </c>
-      <c r="B145" s="90" t="s">
+      <c r="B145" s="91" t="s">
         <v>354</v>
       </c>
-      <c r="C145" s="91" t="s">
+      <c r="C145" s="92" t="s">
         <v>355</v>
       </c>
-      <c r="D145" s="92" t="s">
+      <c r="D145" s="93" t="s">
         <v>356</v>
       </c>
       <c r="E145" s="67" t="s">
@@ -5428,17 +5635,17 @@
       <c r="I145" s="64"/>
     </row>
     <row r="146" customFormat="false" ht="85.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A146" s="89"/>
-      <c r="B146" s="93" t="s">
+      <c r="A146" s="90"/>
+      <c r="B146" s="94" t="s">
         <v>359</v>
       </c>
-      <c r="C146" s="94" t="s">
+      <c r="C146" s="95" t="s">
         <v>360</v>
       </c>
-      <c r="D146" s="95" t="s">
+      <c r="D146" s="96" t="s">
         <v>361</v>
       </c>
-      <c r="E146" s="96" t="s">
+      <c r="E146" s="97" t="s">
         <v>362</v>
       </c>
       <c r="F146" s="29" t="s">
@@ -5449,20 +5656,20 @@
       <c r="I146" s="64"/>
     </row>
     <row r="147" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A147" s="89"/>
-      <c r="B147" s="97" t="s">
+      <c r="A147" s="90"/>
+      <c r="B147" s="98" t="s">
         <v>364</v>
       </c>
-      <c r="C147" s="94" t="s">
+      <c r="C147" s="95" t="s">
         <v>365</v>
       </c>
-      <c r="D147" s="95" t="s">
+      <c r="D147" s="96" t="s">
         <v>366</v>
       </c>
-      <c r="E147" s="98" t="s">
+      <c r="E147" s="99" t="s">
         <v>12</v>
       </c>
-      <c r="F147" s="99" t="s">
+      <c r="F147" s="100" t="s">
         <v>12</v>
       </c>
       <c r="G147" s="64"/>
@@ -5472,21 +5679,21 @@
       <c r="K147" s="64"/>
       <c r="L147" s="64"/>
     </row>
-    <row r="148" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A148" s="89"/>
-      <c r="B148" s="93" t="s">
+    <row r="148" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A148" s="90"/>
+      <c r="B148" s="94" t="s">
         <v>367</v>
       </c>
-      <c r="C148" s="94" t="s">
+      <c r="C148" s="95" t="s">
         <v>365</v>
       </c>
-      <c r="D148" s="95" t="s">
+      <c r="D148" s="96" t="s">
         <v>368</v>
       </c>
-      <c r="E148" s="98" t="s">
+      <c r="E148" s="99" t="s">
         <v>12</v>
       </c>
-      <c r="F148" s="99" t="s">
+      <c r="F148" s="100" t="s">
         <v>12</v>
       </c>
       <c r="G148" s="64"/>
@@ -5496,21 +5703,21 @@
       <c r="K148" s="64"/>
       <c r="L148" s="64"/>
     </row>
-    <row r="149" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A149" s="89"/>
-      <c r="B149" s="100" t="s">
+    <row r="149" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A149" s="90"/>
+      <c r="B149" s="101" t="s">
         <v>304</v>
       </c>
-      <c r="C149" s="101" t="s">
+      <c r="C149" s="102" t="s">
         <v>365</v>
       </c>
-      <c r="D149" s="102" t="s">
+      <c r="D149" s="103" t="s">
         <v>369</v>
       </c>
-      <c r="E149" s="103" t="s">
+      <c r="E149" s="104" t="s">
         <v>12</v>
       </c>
-      <c r="F149" s="104" t="s">
+      <c r="F149" s="105" t="s">
         <v>12</v>
       </c>
       <c r="G149" s="64"/>
@@ -5520,7 +5727,7 @@
       <c r="K149" s="64"/>
       <c r="L149" s="64"/>
     </row>
-    <row r="150" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="150" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="64"/>
       <c r="B150" s="64"/>
       <c r="C150" s="64"/>
@@ -5534,7 +5741,7 @@
       <c r="K150" s="64"/>
       <c r="L150" s="64"/>
     </row>
-    <row r="151" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="151" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="64"/>
       <c r="B151" s="64"/>
       <c r="C151" s="64"/>
@@ -5548,7 +5755,7 @@
       <c r="K151" s="64"/>
       <c r="L151" s="64"/>
     </row>
-    <row r="152" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="152" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="64"/>
       <c r="B152" s="64"/>
       <c r="C152" s="64"/>
@@ -5562,7 +5769,7 @@
       <c r="K152" s="64"/>
       <c r="L152" s="64"/>
     </row>
-    <row r="153" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="153" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="64"/>
       <c r="B153" s="64"/>
       <c r="C153" s="64"/>
@@ -7318,8 +7525,8 @@
     <mergeCell ref="A145:A149"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
update hmi interface to include all other params
</commit_message>
<xml_diff>
--- a/documentation/Tabla_de_registros_HMI_Ivan.xlsx
+++ b/documentation/Tabla_de_registros_HMI_Ivan.xlsx
@@ -8,8 +8,8 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Registros para logica" sheetId="1" state="visible" r:id="rId3"/>
-    <sheet name="Registros" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="Registros para logica" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Registros" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Registros!$A$1:$J$1</definedName>
@@ -26,7 +26,7 @@
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author>Unknown Author</author>
+    <author> </author>
   </authors>
   <commentList>
     <comment ref="B131" authorId="0">
@@ -36,6 +36,7 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">These goes to the HMI, will add the sensor reading to be displayed here, which are the values from IOLink data</t>
         </r>
@@ -46,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="674" uniqueCount="370">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="371">
   <si>
     <t xml:space="preserve">Elemento IOLink</t>
   </si>
@@ -279,9 +280,10 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Cubeta llena entre el 100 y 80 </t>
     </r>
@@ -292,6 +294,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(Lleno</t>
     </r>
@@ -301,6 +304,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">)</t>
     </r>
@@ -312,9 +316,10 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Cubeta entre el 79 y 50 (</t>
     </r>
@@ -325,6 +330,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Medio-alto</t>
     </r>
@@ -334,6 +340,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">)</t>
     </r>
@@ -345,9 +352,10 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Cubeta entre el 49 y 30 (</t>
     </r>
@@ -358,6 +366,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Medio</t>
     </r>
@@ -367,6 +376,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">)</t>
     </r>
@@ -378,9 +388,10 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Cubeta entre el 20 y 10 (</t>
     </r>
@@ -391,6 +402,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Prevacio</t>
     </r>
@@ -400,6 +412,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">)</t>
     </r>
@@ -411,9 +424,10 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Cubeta entre el 5 hacia abajo (2cm) (</t>
     </r>
@@ -424,6 +438,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Vacio</t>
     </r>
@@ -433,6 +448,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">)</t>
     </r>
@@ -1209,139 +1225,40 @@
     <t xml:space="preserve">sensor_material_pressure </t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">HR-0030 – </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">HR-40048</t>
-    </r>
+    <t xml:space="preserve">HR-0030 – HR-40048</t>
   </si>
   <si>
     <t xml:space="preserve">sensor_material_temperature </t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">HR-0031 – </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">HR-40049</t>
-    </r>
+    <t xml:space="preserve">HR-0031 – HR-40049</t>
   </si>
   <si>
     <t xml:space="preserve">sensor_laser_distance </t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">HR-0032 -</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">HR-40050</t>
-    </r>
+    <t xml:space="preserve">HR-0032 -HR-40050</t>
   </si>
   <si>
     <t xml:space="preserve">sensor_pressure_regulator_read_set </t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">HR-0033 – </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">HR-40051</t>
-    </r>
+    <t xml:space="preserve">HR-0033 – HR-40051</t>
   </si>
   <si>
     <t xml:space="preserve">sensor_pressure_regulator_read_real </t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">HR-0034 – </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">HR-40052</t>
-    </r>
+    <t xml:space="preserve">HR-0034 – HR-40052</t>
   </si>
   <si>
     <t xml:space="preserve">sensor_pressure_regulator_valve_read_state </t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">HR-0035 – </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">HR-40053</t>
-    </r>
+    <t xml:space="preserve">HR-0035 – HR-40053</t>
+  </si>
+  <si>
+    <t xml:space="preserve">These are HMI registers</t>
   </si>
   <si>
     <t xml:space="preserve">Datos</t>
@@ -1421,12 +1338,13 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="_-\$* #,##0.00_-;&quot;-$&quot;* #,##0.00_-;_-\$* \-??_-;_-@_-"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="11">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1445,22 +1363,10 @@
     </font>
     <font>
       <sz val="12"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -1468,40 +1374,47 @@
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <u val="single"/>
       <sz val="24"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="16"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="14"/>
+      <color rgb="FFC9211E"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1511,36 +1424,42 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
-        <bgColor rgb="FF993300"/>
+        <bgColor rgb="FFC9211E"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor rgb="FF70AD47"/>
         <bgColor rgb="FF339966"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor rgb="FFFFC000"/>
         <bgColor rgb="FFFF9900"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFF5CE"/>
+        <bgColor rgb="FFFFFFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFD8CE"/>
         <bgColor rgb="FFFFF5CE"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFF5CE"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFD8CE"/>
+        <fgColor rgb="FFFFFFD7"/>
         <bgColor rgb="FFFFF5CE"/>
       </patternFill>
     </fill>
@@ -1795,7 +1714,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="108">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1828,7 +1747,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2056,16 +1975,12 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -2080,10 +1995,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="6" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2096,10 +2007,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2112,10 +2019,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="6" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2124,7 +2027,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2132,11 +2035,15 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2160,20 +2067,44 @@
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="8" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="8" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="8" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="8" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="8" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="8" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="8" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -2184,19 +2115,15 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2231,23 +2158,6 @@
     <cellStyle name="Moneda 2" xfId="20"/>
     <cellStyle name="Moneda 3" xfId="21"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF000000"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -2268,7 +2178,7 @@
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFF5CE"/>
+      <rgbColor rgb="FFFFFFD7"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
@@ -2285,7 +2195,7 @@
       <rgbColor rgb="FF00CCFF"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FFCCFFCC"/>
-      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FFFFF5CE"/>
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
@@ -2302,7 +2212,7 @@
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FFC9211E"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
@@ -2315,114 +2225,8 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Tema de Office">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:srgbClr val="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:srgbClr val="ffffff"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="44546a"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="e7e6e6"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="5b9bd5"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="ed7d31"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="a5a5a5"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="ffc000"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="4472c4"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="70ad47"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0563c1"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="954f72"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme>
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter/>
-        </a:ln>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter/>
-        </a:ln>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -2432,7 +2236,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.57"/>
@@ -2443,8 +2247,8 @@
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2453,29 +2257,29 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:L308"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A127" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H146" activeCellId="0" sqref="H146"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.4453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="26.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="61.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="45.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="34.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="18.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="13.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="20.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="24.14"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="11" style="1" width="11.43"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="11" style="1" width="11.43"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4239,16 +4043,16 @@
       <c r="A74" s="23" t="s">
         <v>100</v>
       </c>
-      <c r="B74" s="67" t="s">
+      <c r="B74" s="8" t="s">
         <v>7</v>
       </c>
       <c r="C74" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="D74" s="68" t="s">
+      <c r="D74" s="67" t="s">
         <v>101</v>
       </c>
-      <c r="E74" s="69" t="s">
+      <c r="E74" s="68" t="s">
         <v>102</v>
       </c>
       <c r="F74" s="64"/>
@@ -4259,82 +4063,82 @@
       <c r="A75" s="23" t="s">
         <v>103</v>
       </c>
-      <c r="B75" s="67" t="s">
+      <c r="B75" s="8" t="s">
         <v>104</v>
       </c>
       <c r="C75" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="D75" s="70" t="s">
+      <c r="D75" s="69" t="s">
         <v>106</v>
       </c>
-      <c r="E75" s="70" t="s">
+      <c r="E75" s="69" t="s">
         <v>107</v>
       </c>
-      <c r="F75" s="71" t="s">
+      <c r="F75" s="29" t="s">
         <v>108</v>
       </c>
-      <c r="G75" s="71"/>
-      <c r="H75" s="71"/>
-      <c r="I75" s="71"/>
-      <c r="J75" s="71"/>
+      <c r="G75" s="29"/>
+      <c r="H75" s="29"/>
+      <c r="I75" s="29"/>
+      <c r="J75" s="29"/>
     </row>
     <row r="76" customFormat="false" ht="43.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="23" t="s">
         <v>109</v>
       </c>
-      <c r="B76" s="67" t="s">
+      <c r="B76" s="8" t="s">
         <v>110</v>
       </c>
       <c r="C76" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="D76" s="70" t="s">
+      <c r="D76" s="69" t="s">
         <v>112</v>
       </c>
-      <c r="E76" s="70" t="s">
+      <c r="E76" s="69" t="s">
         <v>107</v>
       </c>
-      <c r="F76" s="71" t="s">
+      <c r="F76" s="29" t="s">
         <v>113</v>
       </c>
-      <c r="G76" s="71"/>
-      <c r="H76" s="71"/>
-      <c r="I76" s="71"/>
-      <c r="J76" s="71"/>
+      <c r="G76" s="29"/>
+      <c r="H76" s="29"/>
+      <c r="I76" s="29"/>
+      <c r="J76" s="29"/>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="72" t="s">
+      <c r="A77" s="70" t="s">
         <v>114</v>
       </c>
-      <c r="B77" s="73" t="s">
+      <c r="B77" s="71" t="s">
         <v>115</v>
       </c>
       <c r="C77" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="D77" s="70" t="s">
+      <c r="D77" s="69" t="s">
         <v>117</v>
       </c>
-      <c r="E77" s="70" t="s">
+      <c r="E77" s="69" t="s">
         <v>107</v>
       </c>
       <c r="F77" s="64"/>
     </row>
     <row r="78" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="72" t="s">
+      <c r="A78" s="70" t="s">
         <v>118</v>
       </c>
-      <c r="B78" s="73" t="s">
+      <c r="B78" s="71" t="s">
         <v>119</v>
       </c>
       <c r="C78" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="D78" s="70" t="s">
+      <c r="D78" s="69" t="s">
         <v>121</v>
       </c>
-      <c r="E78" s="70" t="s">
+      <c r="E78" s="69" t="s">
         <v>107</v>
       </c>
       <c r="F78" s="64"/>
@@ -4343,16 +4147,16 @@
       <c r="A79" s="28" t="s">
         <v>122</v>
       </c>
-      <c r="B79" s="67" t="s">
+      <c r="B79" s="8" t="s">
         <v>123</v>
       </c>
       <c r="C79" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="D79" s="70" t="s">
+      <c r="D79" s="69" t="s">
         <v>125</v>
       </c>
-      <c r="E79" s="70" t="s">
+      <c r="E79" s="69" t="s">
         <v>107</v>
       </c>
       <c r="F79" s="64"/>
@@ -4361,16 +4165,16 @@
       <c r="A80" s="23" t="s">
         <v>126</v>
       </c>
-      <c r="B80" s="67" t="s">
+      <c r="B80" s="8" t="s">
         <v>127</v>
       </c>
       <c r="C80" s="18" t="s">
         <v>128</v>
       </c>
-      <c r="D80" s="70" t="s">
+      <c r="D80" s="69" t="s">
         <v>129</v>
       </c>
-      <c r="E80" s="70" t="s">
+      <c r="E80" s="69" t="s">
         <v>107</v>
       </c>
       <c r="F80" s="64"/>
@@ -4379,16 +4183,16 @@
       <c r="A81" s="23" t="s">
         <v>130</v>
       </c>
-      <c r="B81" s="67" t="s">
+      <c r="B81" s="8" t="s">
         <v>131</v>
       </c>
       <c r="C81" s="18" t="s">
         <v>132</v>
       </c>
-      <c r="D81" s="70" t="s">
+      <c r="D81" s="69" t="s">
         <v>133</v>
       </c>
-      <c r="E81" s="70" t="s">
+      <c r="E81" s="69" t="s">
         <v>107</v>
       </c>
       <c r="F81" s="64"/>
@@ -4397,16 +4201,16 @@
       <c r="A82" s="23" t="s">
         <v>134</v>
       </c>
-      <c r="B82" s="67" t="s">
+      <c r="B82" s="8" t="s">
         <v>135</v>
       </c>
       <c r="C82" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="D82" s="70" t="s">
+      <c r="D82" s="69" t="s">
         <v>137</v>
       </c>
-      <c r="E82" s="70" t="s">
+      <c r="E82" s="69" t="s">
         <v>138</v>
       </c>
       <c r="F82" s="64"/>
@@ -4415,16 +4219,16 @@
       <c r="A83" s="23" t="s">
         <v>139</v>
       </c>
-      <c r="B83" s="67" t="s">
+      <c r="B83" s="8" t="s">
         <v>140</v>
       </c>
       <c r="C83" s="18" t="s">
         <v>141</v>
       </c>
-      <c r="D83" s="70" t="s">
+      <c r="D83" s="69" t="s">
         <v>142</v>
       </c>
-      <c r="E83" s="70" t="s">
+      <c r="E83" s="69" t="s">
         <v>138</v>
       </c>
       <c r="F83" s="64"/>
@@ -4433,16 +4237,16 @@
       <c r="A84" s="23" t="s">
         <v>143</v>
       </c>
-      <c r="B84" s="67" t="s">
+      <c r="B84" s="8" t="s">
         <v>144</v>
       </c>
       <c r="C84" s="18" t="s">
         <v>145</v>
       </c>
-      <c r="D84" s="70" t="s">
+      <c r="D84" s="69" t="s">
         <v>146</v>
       </c>
-      <c r="E84" s="70" t="s">
+      <c r="E84" s="69" t="s">
         <v>138</v>
       </c>
       <c r="F84" s="64"/>
@@ -4454,16 +4258,16 @@
       <c r="A85" s="23" t="s">
         <v>147</v>
       </c>
-      <c r="B85" s="67" t="s">
+      <c r="B85" s="8" t="s">
         <v>148</v>
       </c>
       <c r="C85" s="18" t="s">
         <v>149</v>
       </c>
-      <c r="D85" s="70" t="s">
+      <c r="D85" s="69" t="s">
         <v>150</v>
       </c>
-      <c r="E85" s="70" t="s">
+      <c r="E85" s="69" t="s">
         <v>138</v>
       </c>
       <c r="F85" s="64"/>
@@ -4475,40 +4279,40 @@
       <c r="A86" s="23" t="s">
         <v>151</v>
       </c>
-      <c r="B86" s="67" t="s">
+      <c r="B86" s="8" t="s">
         <v>152</v>
       </c>
       <c r="C86" s="18" t="s">
         <v>153</v>
       </c>
-      <c r="D86" s="70" t="s">
+      <c r="D86" s="69" t="s">
         <v>154</v>
       </c>
-      <c r="E86" s="70" t="s">
+      <c r="E86" s="69" t="s">
         <v>138</v>
       </c>
-      <c r="F86" s="71" t="s">
+      <c r="F86" s="29" t="s">
         <v>155</v>
       </c>
-      <c r="G86" s="71"/>
-      <c r="H86" s="71"/>
-      <c r="I86" s="71"/>
-      <c r="J86" s="71"/>
+      <c r="G86" s="29"/>
+      <c r="H86" s="29"/>
+      <c r="I86" s="29"/>
+      <c r="J86" s="29"/>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="23" t="s">
         <v>156</v>
       </c>
-      <c r="B87" s="67" t="s">
+      <c r="B87" s="8" t="s">
         <v>157</v>
       </c>
       <c r="C87" s="18" t="s">
         <v>158</v>
       </c>
-      <c r="D87" s="70" t="s">
+      <c r="D87" s="69" t="s">
         <v>159</v>
       </c>
-      <c r="E87" s="70" t="s">
+      <c r="E87" s="69" t="s">
         <v>138</v>
       </c>
       <c r="F87" s="64"/>
@@ -4516,43 +4320,43 @@
       <c r="I87" s="64"/>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="72" t="s">
+      <c r="A88" s="70" t="s">
         <v>160</v>
       </c>
-      <c r="B88" s="73" t="s">
+      <c r="B88" s="71" t="s">
         <v>161</v>
       </c>
       <c r="C88" s="18" t="s">
         <v>162</v>
       </c>
-      <c r="D88" s="74" t="s">
+      <c r="D88" s="72" t="s">
         <v>163</v>
       </c>
-      <c r="E88" s="70" t="s">
+      <c r="E88" s="69" t="s">
         <v>138</v>
       </c>
-      <c r="F88" s="75" t="s">
+      <c r="F88" s="13" t="s">
         <v>164</v>
       </c>
-      <c r="G88" s="75"/>
-      <c r="H88" s="75"/>
-      <c r="I88" s="75"/>
-      <c r="J88" s="75"/>
+      <c r="G88" s="13"/>
+      <c r="H88" s="13"/>
+      <c r="I88" s="13"/>
+      <c r="J88" s="13"/>
     </row>
     <row r="89" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="23" t="s">
         <v>165</v>
       </c>
-      <c r="B89" s="67" t="s">
+      <c r="B89" s="8" t="s">
         <v>166</v>
       </c>
       <c r="C89" s="18" t="s">
         <v>167</v>
       </c>
-      <c r="D89" s="70" t="s">
+      <c r="D89" s="69" t="s">
         <v>168</v>
       </c>
-      <c r="E89" s="70" t="s">
+      <c r="E89" s="69" t="s">
         <v>107</v>
       </c>
       <c r="F89" s="64"/>
@@ -4564,40 +4368,40 @@
       <c r="A90" s="23" t="s">
         <v>169</v>
       </c>
-      <c r="B90" s="67" t="s">
+      <c r="B90" s="8" t="s">
         <v>170</v>
       </c>
       <c r="C90" s="18" t="s">
         <v>171</v>
       </c>
-      <c r="D90" s="70" t="s">
+      <c r="D90" s="69" t="s">
         <v>172</v>
       </c>
-      <c r="E90" s="70" t="s">
+      <c r="E90" s="69" t="s">
         <v>173</v>
       </c>
-      <c r="F90" s="71" t="s">
+      <c r="F90" s="29" t="s">
         <v>174</v>
       </c>
-      <c r="G90" s="71"/>
-      <c r="H90" s="71"/>
-      <c r="I90" s="71"/>
-      <c r="J90" s="71"/>
+      <c r="G90" s="29"/>
+      <c r="H90" s="29"/>
+      <c r="I90" s="29"/>
+      <c r="J90" s="29"/>
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="72" t="s">
+      <c r="A91" s="70" t="s">
         <v>175</v>
       </c>
-      <c r="B91" s="73" t="s">
+      <c r="B91" s="71" t="s">
         <v>176</v>
       </c>
       <c r="C91" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="D91" s="76" t="s">
+      <c r="D91" s="73" t="s">
         <v>178</v>
       </c>
-      <c r="E91" s="70" t="s">
+      <c r="E91" s="69" t="s">
         <v>179</v>
       </c>
       <c r="F91" s="64"/>
@@ -4606,19 +4410,19 @@
       <c r="I91" s="64"/>
     </row>
     <row r="92" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="72" t="s">
+      <c r="A92" s="70" t="s">
         <v>118</v>
       </c>
-      <c r="B92" s="73" t="s">
+      <c r="B92" s="71" t="s">
         <v>180</v>
       </c>
       <c r="C92" s="18" t="s">
         <v>181</v>
       </c>
-      <c r="D92" s="70" t="s">
+      <c r="D92" s="69" t="s">
         <v>182</v>
       </c>
-      <c r="E92" s="70" t="s">
+      <c r="E92" s="69" t="s">
         <v>179</v>
       </c>
       <c r="F92" s="64"/>
@@ -4627,19 +4431,19 @@
       <c r="I92" s="64"/>
     </row>
     <row r="93" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="77" t="s">
+      <c r="A93" s="74" t="s">
         <v>183</v>
       </c>
-      <c r="B93" s="73" t="s">
+      <c r="B93" s="71" t="s">
         <v>184</v>
       </c>
       <c r="C93" s="18" t="s">
         <v>185</v>
       </c>
-      <c r="D93" s="70" t="s">
+      <c r="D93" s="69" t="s">
         <v>186</v>
       </c>
-      <c r="E93" s="70" t="s">
+      <c r="E93" s="69" t="s">
         <v>179</v>
       </c>
       <c r="F93" s="64"/>
@@ -4648,19 +4452,19 @@
       <c r="I93" s="64"/>
     </row>
     <row r="94" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="78" t="s">
+      <c r="A94" s="75" t="s">
         <v>187</v>
       </c>
-      <c r="B94" s="73" t="s">
+      <c r="B94" s="71" t="s">
         <v>188</v>
       </c>
       <c r="C94" s="18" t="s">
         <v>189</v>
       </c>
-      <c r="D94" s="70" t="s">
+      <c r="D94" s="69" t="s">
         <v>190</v>
       </c>
-      <c r="E94" s="70" t="s">
+      <c r="E94" s="69" t="s">
         <v>179</v>
       </c>
       <c r="F94" s="64"/>
@@ -4672,16 +4476,16 @@
       <c r="A95" s="23" t="s">
         <v>191</v>
       </c>
-      <c r="B95" s="67" t="s">
+      <c r="B95" s="8" t="s">
         <v>192</v>
       </c>
       <c r="C95" s="18" t="s">
         <v>193</v>
       </c>
-      <c r="D95" s="70" t="s">
+      <c r="D95" s="69" t="s">
         <v>194</v>
       </c>
-      <c r="E95" s="70" t="s">
+      <c r="E95" s="69" t="s">
         <v>179</v>
       </c>
       <c r="F95" s="64"/>
@@ -4693,16 +4497,16 @@
       <c r="A96" s="23" t="s">
         <v>195</v>
       </c>
-      <c r="B96" s="67" t="s">
+      <c r="B96" s="8" t="s">
         <v>196</v>
       </c>
       <c r="C96" s="18" t="s">
         <v>197</v>
       </c>
-      <c r="D96" s="70" t="s">
+      <c r="D96" s="69" t="s">
         <v>198</v>
       </c>
-      <c r="E96" s="70" t="s">
+      <c r="E96" s="69" t="s">
         <v>179</v>
       </c>
       <c r="F96" s="64"/>
@@ -4714,16 +4518,16 @@
       <c r="A97" s="23" t="s">
         <v>199</v>
       </c>
-      <c r="B97" s="67" t="s">
+      <c r="B97" s="8" t="s">
         <v>200</v>
       </c>
       <c r="C97" s="18" t="s">
         <v>201</v>
       </c>
-      <c r="D97" s="70" t="s">
+      <c r="D97" s="69" t="s">
         <v>202</v>
       </c>
-      <c r="E97" s="70" t="s">
+      <c r="E97" s="69" t="s">
         <v>179</v>
       </c>
       <c r="F97" s="64"/>
@@ -4735,16 +4539,16 @@
       <c r="A98" s="23" t="s">
         <v>203</v>
       </c>
-      <c r="B98" s="67" t="s">
+      <c r="B98" s="8" t="s">
         <v>204</v>
       </c>
       <c r="C98" s="18" t="s">
         <v>205</v>
       </c>
-      <c r="D98" s="74" t="s">
+      <c r="D98" s="72" t="s">
         <v>206</v>
       </c>
-      <c r="E98" s="70" t="s">
+      <c r="E98" s="69" t="s">
         <v>179</v>
       </c>
       <c r="F98" s="64"/>
@@ -4756,16 +4560,16 @@
       <c r="A99" s="23" t="s">
         <v>207</v>
       </c>
-      <c r="B99" s="67" t="s">
+      <c r="B99" s="8" t="s">
         <v>208</v>
       </c>
       <c r="C99" s="18" t="s">
         <v>209</v>
       </c>
-      <c r="D99" s="70" t="s">
+      <c r="D99" s="69" t="s">
         <v>210</v>
       </c>
-      <c r="E99" s="70" t="s">
+      <c r="E99" s="69" t="s">
         <v>179</v>
       </c>
       <c r="F99" s="64"/>
@@ -4777,40 +4581,40 @@
       <c r="A100" s="23" t="s">
         <v>103</v>
       </c>
-      <c r="B100" s="67" t="s">
+      <c r="B100" s="8" t="s">
         <v>211</v>
       </c>
       <c r="C100" s="18" t="s">
         <v>212</v>
       </c>
-      <c r="D100" s="70" t="s">
+      <c r="D100" s="69" t="s">
         <v>213</v>
       </c>
-      <c r="E100" s="70" t="s">
+      <c r="E100" s="69" t="s">
         <v>179</v>
       </c>
-      <c r="F100" s="71" t="s">
+      <c r="F100" s="29" t="s">
         <v>214</v>
       </c>
-      <c r="G100" s="71"/>
-      <c r="H100" s="71"/>
-      <c r="I100" s="71"/>
-      <c r="J100" s="71"/>
+      <c r="G100" s="29"/>
+      <c r="H100" s="29"/>
+      <c r="I100" s="29"/>
+      <c r="J100" s="29"/>
     </row>
     <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="23" t="s">
         <v>130</v>
       </c>
-      <c r="B101" s="67" t="s">
+      <c r="B101" s="8" t="s">
         <v>215</v>
       </c>
       <c r="C101" s="18" t="s">
         <v>216</v>
       </c>
-      <c r="D101" s="70" t="s">
+      <c r="D101" s="69" t="s">
         <v>217</v>
       </c>
-      <c r="E101" s="70" t="s">
+      <c r="E101" s="69" t="s">
         <v>179</v>
       </c>
       <c r="F101" s="64"/>
@@ -4819,19 +4623,19 @@
       <c r="I101" s="64"/>
     </row>
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="79" t="s">
+      <c r="A102" s="23" t="s">
         <v>218</v>
       </c>
-      <c r="B102" s="67" t="s">
+      <c r="B102" s="8" t="s">
         <v>219</v>
       </c>
       <c r="C102" s="18" t="s">
         <v>220</v>
       </c>
-      <c r="D102" s="70" t="s">
+      <c r="D102" s="69" t="s">
         <v>221</v>
       </c>
-      <c r="E102" s="70" t="s">
+      <c r="E102" s="69" t="s">
         <v>179</v>
       </c>
       <c r="F102" s="64"/>
@@ -4843,16 +4647,16 @@
       <c r="A103" s="23" t="s">
         <v>222</v>
       </c>
-      <c r="B103" s="67" t="s">
+      <c r="B103" s="8" t="s">
         <v>223</v>
       </c>
       <c r="C103" s="18" t="s">
         <v>224</v>
       </c>
-      <c r="D103" s="70" t="s">
+      <c r="D103" s="69" t="s">
         <v>225</v>
       </c>
-      <c r="E103" s="70" t="s">
+      <c r="E103" s="69" t="s">
         <v>226</v>
       </c>
       <c r="F103" s="64"/>
@@ -4864,16 +4668,16 @@
       <c r="A104" s="23" t="s">
         <v>227</v>
       </c>
-      <c r="B104" s="67" t="s">
+      <c r="B104" s="8" t="s">
         <v>228</v>
       </c>
       <c r="C104" s="18" t="s">
         <v>229</v>
       </c>
-      <c r="D104" s="70" t="s">
+      <c r="D104" s="69" t="s">
         <v>230</v>
       </c>
-      <c r="E104" s="70" t="s">
+      <c r="E104" s="69" t="s">
         <v>226</v>
       </c>
       <c r="F104" s="64"/>
@@ -4885,16 +4689,16 @@
       <c r="A105" s="23" t="s">
         <v>147</v>
       </c>
-      <c r="B105" s="67" t="s">
+      <c r="B105" s="8" t="s">
         <v>231</v>
       </c>
       <c r="C105" s="18" t="s">
         <v>232</v>
       </c>
-      <c r="D105" s="70" t="s">
+      <c r="D105" s="69" t="s">
         <v>150</v>
       </c>
-      <c r="E105" s="70" t="s">
+      <c r="E105" s="69" t="s">
         <v>226</v>
       </c>
       <c r="F105" s="64"/>
@@ -4903,19 +4707,19 @@
       <c r="I105" s="64"/>
     </row>
     <row r="106" customFormat="false" ht="74.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A106" s="80" t="s">
+      <c r="A106" s="76" t="s">
         <v>233</v>
       </c>
-      <c r="B106" s="73" t="s">
+      <c r="B106" s="71" t="s">
         <v>234</v>
       </c>
       <c r="C106" s="18" t="s">
         <v>235</v>
       </c>
-      <c r="D106" s="67" t="s">
+      <c r="D106" s="8" t="s">
         <v>236</v>
       </c>
-      <c r="E106" s="70" t="s">
+      <c r="E106" s="69" t="s">
         <v>237</v>
       </c>
       <c r="F106" s="8" t="s">
@@ -4927,70 +4731,70 @@
       <c r="J106" s="8"/>
     </row>
     <row r="107" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="77" t="s">
+      <c r="A107" s="74" t="s">
         <v>239</v>
       </c>
-      <c r="B107" s="73" t="s">
+      <c r="B107" s="71" t="s">
         <v>240</v>
       </c>
       <c r="C107" s="18" t="s">
         <v>241</v>
       </c>
-      <c r="D107" s="67" t="s">
+      <c r="D107" s="8" t="s">
         <v>242</v>
       </c>
-      <c r="E107" s="70" t="s">
+      <c r="E107" s="69" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A108" s="72" t="s">
+      <c r="A108" s="70" t="s">
         <v>243</v>
       </c>
-      <c r="B108" s="73" t="s">
+      <c r="B108" s="71" t="s">
         <v>244</v>
       </c>
       <c r="C108" s="18" t="s">
         <v>245</v>
       </c>
-      <c r="D108" s="67" t="s">
+      <c r="D108" s="8" t="s">
         <v>246</v>
       </c>
-      <c r="E108" s="70" t="s">
+      <c r="E108" s="69" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A109" s="72" t="s">
+      <c r="A109" s="70" t="s">
         <v>247</v>
       </c>
-      <c r="B109" s="73" t="s">
+      <c r="B109" s="71" t="s">
         <v>248</v>
       </c>
       <c r="C109" s="18" t="s">
         <v>249</v>
       </c>
-      <c r="D109" s="67" t="s">
+      <c r="D109" s="8" t="s">
         <v>250</v>
       </c>
-      <c r="E109" s="70" t="s">
+      <c r="E109" s="69" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="142.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A110" s="81" t="s">
+      <c r="A110" s="77" t="s">
         <v>251</v>
       </c>
-      <c r="B110" s="67" t="s">
+      <c r="B110" s="8" t="s">
         <v>252</v>
       </c>
       <c r="C110" s="18" t="s">
         <v>253</v>
       </c>
-      <c r="D110" s="67" t="s">
+      <c r="D110" s="8" t="s">
         <v>254</v>
       </c>
-      <c r="E110" s="70" t="s">
+      <c r="E110" s="69" t="s">
         <v>255</v>
       </c>
       <c r="F110" s="8" t="s">
@@ -5002,19 +4806,19 @@
       <c r="J110" s="8"/>
     </row>
     <row r="111" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A111" s="81" t="s">
+      <c r="A111" s="77" t="s">
         <v>257</v>
       </c>
-      <c r="B111" s="67" t="s">
+      <c r="B111" s="8" t="s">
         <v>258</v>
       </c>
       <c r="C111" s="18" t="s">
         <v>259</v>
       </c>
-      <c r="D111" s="67" t="s">
+      <c r="D111" s="8" t="s">
         <v>260</v>
       </c>
-      <c r="E111" s="70" t="s">
+      <c r="E111" s="69" t="s">
         <v>255</v>
       </c>
       <c r="F111" s="64"/>
@@ -5026,16 +4830,16 @@
       <c r="A112" s="23" t="s">
         <v>261</v>
       </c>
-      <c r="B112" s="67" t="s">
+      <c r="B112" s="8" t="s">
         <v>262</v>
       </c>
       <c r="C112" s="18" t="s">
         <v>263</v>
       </c>
-      <c r="D112" s="67" t="s">
+      <c r="D112" s="8" t="s">
         <v>198</v>
       </c>
-      <c r="E112" s="70" t="s">
+      <c r="E112" s="69" t="s">
         <v>255</v>
       </c>
       <c r="F112" s="8" t="s">
@@ -5049,16 +4853,16 @@
       <c r="A113" s="23" t="s">
         <v>265</v>
       </c>
-      <c r="B113" s="67" t="s">
+      <c r="B113" s="8" t="s">
         <v>266</v>
       </c>
       <c r="C113" s="18" t="s">
         <v>267</v>
       </c>
-      <c r="D113" s="67" t="s">
+      <c r="D113" s="8" t="s">
         <v>202</v>
       </c>
-      <c r="E113" s="70" t="s">
+      <c r="E113" s="69" t="s">
         <v>255</v>
       </c>
       <c r="G113" s="64"/>
@@ -5066,10 +4870,10 @@
       <c r="I113" s="64"/>
     </row>
     <row r="114" customFormat="false" ht="26.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A114" s="81" t="s">
+      <c r="A114" s="77" t="s">
         <v>268</v>
       </c>
-      <c r="B114" s="67" t="s">
+      <c r="B114" s="8" t="s">
         <v>269</v>
       </c>
       <c r="C114" s="18" t="s">
@@ -5078,31 +4882,31 @@
       <c r="D114" s="21" t="s">
         <v>271</v>
       </c>
-      <c r="E114" s="70" t="s">
+      <c r="E114" s="69" t="s">
         <v>255</v>
       </c>
-      <c r="F114" s="82" t="s">
+      <c r="F114" s="78" t="s">
         <v>272</v>
       </c>
-      <c r="G114" s="82"/>
-      <c r="H114" s="82"/>
-      <c r="I114" s="82"/>
-      <c r="J114" s="82"/>
+      <c r="G114" s="78"/>
+      <c r="H114" s="78"/>
+      <c r="I114" s="78"/>
+      <c r="J114" s="78"/>
     </row>
     <row r="115" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A115" s="23" t="s">
         <v>273</v>
       </c>
-      <c r="B115" s="67" t="s">
+      <c r="B115" s="8" t="s">
         <v>274</v>
       </c>
       <c r="C115" s="18" t="s">
         <v>275</v>
       </c>
-      <c r="D115" s="70" t="s">
+      <c r="D115" s="69" t="s">
         <v>221</v>
       </c>
-      <c r="E115" s="70" t="s">
+      <c r="E115" s="69" t="s">
         <v>255</v>
       </c>
       <c r="F115" s="64"/>
@@ -5111,19 +4915,19 @@
       <c r="I115" s="64"/>
     </row>
     <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A116" s="72" t="s">
+      <c r="A116" s="70" t="s">
         <v>276</v>
       </c>
-      <c r="B116" s="73" t="s">
+      <c r="B116" s="71" t="s">
         <v>277</v>
       </c>
       <c r="C116" s="18" t="s">
         <v>278</v>
       </c>
-      <c r="D116" s="67" t="s">
+      <c r="D116" s="8" t="s">
         <v>279</v>
       </c>
-      <c r="E116" s="70" t="s">
+      <c r="E116" s="69" t="s">
         <v>280</v>
       </c>
       <c r="F116" s="64"/>
@@ -5132,19 +4936,19 @@
       <c r="I116" s="64"/>
     </row>
     <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A117" s="72" t="s">
+      <c r="A117" s="70" t="s">
         <v>281</v>
       </c>
-      <c r="B117" s="73" t="s">
+      <c r="B117" s="71" t="s">
         <v>282</v>
       </c>
       <c r="C117" s="18" t="s">
         <v>283</v>
       </c>
-      <c r="D117" s="67" t="s">
+      <c r="D117" s="8" t="s">
         <v>284</v>
       </c>
-      <c r="E117" s="70" t="s">
+      <c r="E117" s="69" t="s">
         <v>280</v>
       </c>
       <c r="F117" s="64"/>
@@ -5153,19 +4957,19 @@
       <c r="I117" s="64"/>
     </row>
     <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A118" s="72" t="s">
+      <c r="A118" s="70" t="s">
         <v>285</v>
       </c>
-      <c r="B118" s="73" t="s">
+      <c r="B118" s="71" t="s">
         <v>286</v>
       </c>
       <c r="C118" s="18" t="s">
         <v>287</v>
       </c>
-      <c r="D118" s="67" t="s">
+      <c r="D118" s="8" t="s">
         <v>288</v>
       </c>
-      <c r="E118" s="70" t="s">
+      <c r="E118" s="69" t="s">
         <v>280</v>
       </c>
       <c r="F118" s="64"/>
@@ -5174,19 +4978,19 @@
       <c r="I118" s="64"/>
     </row>
     <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A119" s="72" t="s">
+      <c r="A119" s="70" t="s">
         <v>289</v>
       </c>
-      <c r="B119" s="73" t="s">
+      <c r="B119" s="71" t="s">
         <v>290</v>
       </c>
       <c r="C119" s="18" t="s">
         <v>291</v>
       </c>
-      <c r="D119" s="67" t="s">
+      <c r="D119" s="8" t="s">
         <v>292</v>
       </c>
-      <c r="E119" s="70" t="s">
+      <c r="E119" s="69" t="s">
         <v>280</v>
       </c>
       <c r="F119" s="64"/>
@@ -5195,19 +4999,19 @@
       <c r="I119" s="64"/>
     </row>
     <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A120" s="72" t="s">
+      <c r="A120" s="70" t="s">
         <v>293</v>
       </c>
-      <c r="B120" s="73" t="s">
+      <c r="B120" s="71" t="s">
         <v>294</v>
       </c>
       <c r="C120" s="18" t="s">
         <v>295</v>
       </c>
-      <c r="D120" s="67" t="s">
+      <c r="D120" s="8" t="s">
         <v>296</v>
       </c>
-      <c r="E120" s="70" t="s">
+      <c r="E120" s="69" t="s">
         <v>280</v>
       </c>
       <c r="F120" s="8"/>
@@ -5217,19 +5021,19 @@
       <c r="J120" s="8"/>
     </row>
     <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A121" s="72" t="s">
+      <c r="A121" s="70" t="s">
         <v>297</v>
       </c>
-      <c r="B121" s="73" t="s">
+      <c r="B121" s="71" t="s">
         <v>298</v>
       </c>
       <c r="C121" s="18" t="s">
         <v>299</v>
       </c>
-      <c r="D121" s="67" t="s">
+      <c r="D121" s="8" t="s">
         <v>300</v>
       </c>
-      <c r="E121" s="70" t="s">
+      <c r="E121" s="69" t="s">
         <v>280</v>
       </c>
       <c r="F121" s="64"/>
@@ -5238,19 +5042,19 @@
       <c r="I121" s="64"/>
     </row>
     <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A122" s="72" t="s">
+      <c r="A122" s="70" t="s">
         <v>301</v>
       </c>
-      <c r="B122" s="73" t="s">
+      <c r="B122" s="71" t="s">
         <v>302</v>
       </c>
       <c r="C122" s="18" t="s">
         <v>303</v>
       </c>
-      <c r="D122" s="67" t="s">
+      <c r="D122" s="8" t="s">
         <v>304</v>
       </c>
-      <c r="E122" s="70" t="s">
+      <c r="E122" s="69" t="s">
         <v>280</v>
       </c>
       <c r="F122" s="64"/>
@@ -5262,16 +5066,16 @@
       <c r="A123" s="23" t="s">
         <v>305</v>
       </c>
-      <c r="B123" s="67" t="s">
+      <c r="B123" s="8" t="s">
         <v>306</v>
       </c>
       <c r="C123" s="18" t="s">
         <v>307</v>
       </c>
-      <c r="D123" s="67" t="s">
+      <c r="D123" s="8" t="s">
         <v>308</v>
       </c>
-      <c r="E123" s="70" t="s">
+      <c r="E123" s="69" t="s">
         <v>280</v>
       </c>
       <c r="F123" s="64"/>
@@ -5283,16 +5087,16 @@
       <c r="A124" s="23" t="s">
         <v>309</v>
       </c>
-      <c r="B124" s="67" t="s">
+      <c r="B124" s="8" t="s">
         <v>310</v>
       </c>
       <c r="C124" s="18" t="s">
         <v>311</v>
       </c>
-      <c r="D124" s="67" t="s">
+      <c r="D124" s="8" t="s">
         <v>312</v>
       </c>
-      <c r="E124" s="70" t="s">
+      <c r="E124" s="69" t="s">
         <v>280</v>
       </c>
       <c r="F124" s="64"/>
@@ -5304,16 +5108,16 @@
       <c r="A125" s="23" t="s">
         <v>313</v>
       </c>
-      <c r="B125" s="67" t="s">
+      <c r="B125" s="8" t="s">
         <v>314</v>
       </c>
       <c r="C125" s="18" t="s">
         <v>315</v>
       </c>
-      <c r="D125" s="67" t="s">
+      <c r="D125" s="8" t="s">
         <v>316</v>
       </c>
-      <c r="E125" s="70" t="s">
+      <c r="E125" s="69" t="s">
         <v>280</v>
       </c>
       <c r="F125" s="64"/>
@@ -5322,19 +5126,19 @@
       <c r="I125" s="64"/>
     </row>
     <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A126" s="72" t="s">
+      <c r="A126" s="70" t="s">
         <v>317</v>
       </c>
-      <c r="B126" s="73" t="s">
+      <c r="B126" s="71" t="s">
         <v>318</v>
       </c>
       <c r="C126" s="18" t="s">
         <v>319</v>
       </c>
-      <c r="D126" s="67" t="s">
+      <c r="D126" s="8" t="s">
         <v>320</v>
       </c>
-      <c r="E126" s="70" t="s">
+      <c r="E126" s="69" t="s">
         <v>321</v>
       </c>
       <c r="F126" s="64"/>
@@ -5343,19 +5147,19 @@
       <c r="I126" s="64"/>
     </row>
     <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A127" s="72" t="s">
+      <c r="A127" s="70" t="s">
         <v>322</v>
       </c>
-      <c r="B127" s="73" t="s">
+      <c r="B127" s="71" t="s">
         <v>323</v>
       </c>
       <c r="C127" s="18" t="s">
         <v>324</v>
       </c>
-      <c r="D127" s="67" t="s">
+      <c r="D127" s="8" t="s">
         <v>325</v>
       </c>
-      <c r="E127" s="70" t="s">
+      <c r="E127" s="69" t="s">
         <v>321</v>
       </c>
       <c r="F127" s="64"/>
@@ -5364,19 +5168,19 @@
       <c r="I127" s="64"/>
     </row>
     <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A128" s="72" t="s">
+      <c r="A128" s="70" t="s">
         <v>326</v>
       </c>
-      <c r="B128" s="73" t="s">
+      <c r="B128" s="71" t="s">
         <v>327</v>
       </c>
       <c r="C128" s="18" t="s">
         <v>328</v>
       </c>
-      <c r="D128" s="67" t="s">
+      <c r="D128" s="8" t="s">
         <v>329</v>
       </c>
-      <c r="E128" s="70" t="s">
+      <c r="E128" s="69" t="s">
         <v>321</v>
       </c>
       <c r="F128" s="64"/>
@@ -5385,19 +5189,19 @@
       <c r="I128" s="64"/>
     </row>
     <row r="129" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A129" s="83" t="s">
+      <c r="A129" s="79" t="s">
         <v>330</v>
       </c>
-      <c r="B129" s="73" t="s">
+      <c r="B129" s="71" t="s">
         <v>331</v>
       </c>
       <c r="C129" s="18" t="s">
         <v>332</v>
       </c>
-      <c r="D129" s="67" t="s">
+      <c r="D129" s="8" t="s">
         <v>333</v>
       </c>
-      <c r="E129" s="70" t="s">
+      <c r="E129" s="69" t="s">
         <v>321</v>
       </c>
       <c r="F129" s="64"/>
@@ -5406,19 +5210,19 @@
       <c r="I129" s="64"/>
     </row>
     <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A130" s="72" t="s">
+      <c r="A130" s="70" t="s">
         <v>334</v>
       </c>
-      <c r="B130" s="73" t="s">
+      <c r="B130" s="71" t="s">
         <v>335</v>
       </c>
       <c r="C130" s="18" t="s">
         <v>336</v>
       </c>
-      <c r="D130" s="67" t="s">
+      <c r="D130" s="8" t="s">
         <v>337</v>
       </c>
-      <c r="E130" s="70" t="s">
+      <c r="E130" s="69" t="s">
         <v>321</v>
       </c>
       <c r="F130" s="64"/>
@@ -5427,10 +5231,10 @@
       <c r="I130" s="64"/>
     </row>
     <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A131" s="84" t="s">
+      <c r="A131" s="80" t="s">
         <v>338</v>
       </c>
-      <c r="B131" s="85" t="s">
+      <c r="B131" s="81" t="s">
         <v>339</v>
       </c>
       <c r="C131" s="64"/>
@@ -5442,10 +5246,10 @@
       <c r="I131" s="64"/>
     </row>
     <row r="132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A132" s="84" t="s">
+      <c r="A132" s="80" t="s">
         <v>340</v>
       </c>
-      <c r="B132" s="85" t="s">
+      <c r="B132" s="81" t="s">
         <v>341</v>
       </c>
       <c r="C132" s="64"/>
@@ -5457,10 +5261,10 @@
       <c r="I132" s="64"/>
     </row>
     <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A133" s="84" t="s">
+      <c r="A133" s="80" t="s">
         <v>342</v>
       </c>
-      <c r="B133" s="85" t="s">
+      <c r="B133" s="81" t="s">
         <v>343</v>
       </c>
       <c r="C133" s="64"/>
@@ -5472,10 +5276,10 @@
       <c r="I133" s="64"/>
     </row>
     <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A134" s="84" t="s">
+      <c r="A134" s="80" t="s">
         <v>344</v>
       </c>
-      <c r="B134" s="85" t="s">
+      <c r="B134" s="81" t="s">
         <v>345</v>
       </c>
       <c r="C134" s="64"/>
@@ -5487,10 +5291,10 @@
       <c r="I134" s="64"/>
     </row>
     <row r="135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A135" s="84" t="s">
+      <c r="A135" s="80" t="s">
         <v>346</v>
       </c>
-      <c r="B135" s="85" t="s">
+      <c r="B135" s="81" t="s">
         <v>347</v>
       </c>
       <c r="C135" s="64"/>
@@ -5502,10 +5306,10 @@
       <c r="I135" s="64"/>
     </row>
     <row r="136" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A136" s="84" t="s">
+      <c r="A136" s="80" t="s">
         <v>348</v>
       </c>
-      <c r="B136" s="85" t="s">
+      <c r="B136" s="81" t="s">
         <v>349</v>
       </c>
       <c r="C136" s="64"/>
@@ -5568,9 +5372,11 @@
       <c r="H141" s="64"/>
       <c r="I141" s="64"/>
     </row>
-    <row r="142" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="142" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="64"/>
-      <c r="B142" s="64"/>
+      <c r="B142" s="82" t="s">
+        <v>350</v>
+      </c>
       <c r="C142" s="64"/>
       <c r="D142" s="64"/>
       <c r="E142" s="64"/>
@@ -5580,17 +5386,17 @@
       <c r="I142" s="64"/>
     </row>
     <row r="143" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A143" s="86"/>
-      <c r="B143" s="87" t="s">
-        <v>350</v>
-      </c>
-      <c r="C143" s="87" t="s">
+      <c r="A143" s="83"/>
+      <c r="B143" s="84" t="s">
         <v>351</v>
       </c>
-      <c r="D143" s="88" t="s">
+      <c r="C143" s="84" t="s">
         <v>352</v>
       </c>
-      <c r="E143" s="67" t="s">
+      <c r="D143" s="85" t="s">
+        <v>353</v>
+      </c>
+      <c r="E143" s="8" t="s">
         <v>7</v>
       </c>
       <c r="F143" s="29" t="s">
@@ -5601,7 +5407,7 @@
       <c r="I143" s="64"/>
     </row>
     <row r="144" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A144" s="89"/>
+      <c r="A144" s="86"/>
       <c r="B144" s="64"/>
       <c r="C144" s="64"/>
       <c r="D144" s="64"/>
@@ -5612,64 +5418,64 @@
       <c r="I144" s="64"/>
     </row>
     <row r="145" customFormat="false" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A145" s="90" t="s">
-        <v>353</v>
-      </c>
-      <c r="B145" s="91" t="s">
+      <c r="A145" s="87" t="s">
         <v>354</v>
       </c>
-      <c r="C145" s="92" t="s">
+      <c r="B145" s="88" t="s">
         <v>355</v>
       </c>
-      <c r="D145" s="93" t="s">
+      <c r="C145" s="89" t="s">
         <v>356</v>
       </c>
-      <c r="E145" s="67" t="s">
+      <c r="D145" s="90" t="s">
         <v>357</v>
       </c>
-      <c r="F145" s="29" t="s">
+      <c r="E145" s="91" t="s">
         <v>358</v>
+      </c>
+      <c r="F145" s="92" t="s">
+        <v>359</v>
       </c>
       <c r="G145" s="64"/>
       <c r="H145" s="64"/>
       <c r="I145" s="64"/>
     </row>
     <row r="146" customFormat="false" ht="85.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A146" s="90"/>
-      <c r="B146" s="94" t="s">
-        <v>359</v>
-      </c>
-      <c r="C146" s="95" t="s">
+      <c r="A146" s="87"/>
+      <c r="B146" s="93" t="s">
         <v>360</v>
       </c>
-      <c r="D146" s="96" t="s">
+      <c r="C146" s="94" t="s">
         <v>361</v>
       </c>
-      <c r="E146" s="97" t="s">
+      <c r="D146" s="95" t="s">
         <v>362</v>
       </c>
-      <c r="F146" s="29" t="s">
+      <c r="E146" s="96" t="s">
         <v>363</v>
+      </c>
+      <c r="F146" s="92" t="s">
+        <v>364</v>
       </c>
       <c r="G146" s="64"/>
       <c r="H146" s="64"/>
       <c r="I146" s="64"/>
     </row>
     <row r="147" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A147" s="90"/>
-      <c r="B147" s="98" t="s">
-        <v>364</v>
-      </c>
-      <c r="C147" s="95" t="s">
+      <c r="A147" s="87"/>
+      <c r="B147" s="97" t="s">
         <v>365</v>
       </c>
-      <c r="D147" s="96" t="s">
+      <c r="C147" s="98" t="s">
         <v>366</v>
       </c>
-      <c r="E147" s="99" t="s">
+      <c r="D147" s="99" t="s">
+        <v>367</v>
+      </c>
+      <c r="E147" s="100" t="s">
         <v>12</v>
       </c>
-      <c r="F147" s="100" t="s">
+      <c r="F147" s="101" t="s">
         <v>12</v>
       </c>
       <c r="G147" s="64"/>
@@ -5680,20 +5486,20 @@
       <c r="L147" s="64"/>
     </row>
     <row r="148" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A148" s="90"/>
-      <c r="B148" s="94" t="s">
-        <v>367</v>
-      </c>
-      <c r="C148" s="95" t="s">
-        <v>365</v>
-      </c>
-      <c r="D148" s="96" t="s">
+      <c r="A148" s="87"/>
+      <c r="B148" s="102" t="s">
         <v>368</v>
       </c>
-      <c r="E148" s="99" t="s">
+      <c r="C148" s="98" t="s">
+        <v>366</v>
+      </c>
+      <c r="D148" s="99" t="s">
+        <v>369</v>
+      </c>
+      <c r="E148" s="100" t="s">
         <v>12</v>
       </c>
-      <c r="F148" s="100" t="s">
+      <c r="F148" s="101" t="s">
         <v>12</v>
       </c>
       <c r="G148" s="64"/>
@@ -5704,20 +5510,20 @@
       <c r="L148" s="64"/>
     </row>
     <row r="149" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A149" s="90"/>
-      <c r="B149" s="101" t="s">
+      <c r="A149" s="87"/>
+      <c r="B149" s="103" t="s">
         <v>304</v>
       </c>
-      <c r="C149" s="102" t="s">
-        <v>365</v>
-      </c>
-      <c r="D149" s="103" t="s">
-        <v>369</v>
-      </c>
-      <c r="E149" s="104" t="s">
+      <c r="C149" s="104" t="s">
+        <v>366</v>
+      </c>
+      <c r="D149" s="105" t="s">
+        <v>370</v>
+      </c>
+      <c r="E149" s="106" t="s">
         <v>12</v>
       </c>
-      <c r="F149" s="105" t="s">
+      <c r="F149" s="107" t="s">
         <v>12</v>
       </c>
       <c r="G149" s="64"/>
@@ -7525,8 +7331,8 @@
     <mergeCell ref="A145:A149"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
create hmi status message
</commit_message>
<xml_diff>
--- a/documentation/Tabla_de_registros_HMI_Ivan.xlsx
+++ b/documentation/Tabla_de_registros_HMI_Ivan.xlsx
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="374">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="375">
   <si>
     <t xml:space="preserve">Elemento IOLink</t>
   </si>
@@ -1134,6 +1134,11 @@
   </si>
   <si>
     <t xml:space="preserve">Selecciona el volumen de la cubeta 19L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">this seems to save the 
+bucket size so we don’t need 
+HR-0021</t>
   </si>
   <si>
     <t xml:space="preserve">Botón Volumen 2</t>
@@ -1437,7 +1442,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1478,6 +1483,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFF5CE"/>
         <bgColor rgb="FFFFFFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFAA95"/>
+        <bgColor rgb="FFFF8080"/>
       </patternFill>
     </fill>
     <fill>
@@ -1737,7 +1748,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="111">
+  <cellXfs count="112">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2062,6 +2073,10 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="7" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2070,11 +2085,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="10" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2232,7 +2247,7 @@
       <rgbColor rgb="FFCCFFCC"/>
       <rgbColor rgb="FFFFF5CE"/>
       <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFFFAA95"/>
       <rgbColor rgb="FFCC99FF"/>
       <rgbColor rgb="FFFFD8CE"/>
       <rgbColor rgb="FF3366FF"/>
@@ -2268,7 +2283,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="F127:F129 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2298,8 +2313,8 @@
   </sheetPr>
   <dimension ref="A1:L309"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A54" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G71" activeCellId="0" sqref="G71"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A110" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F129" activeCellId="0" sqref="F127:F129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.4453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5097,7 +5112,7 @@
       <c r="H122" s="66"/>
       <c r="I122" s="66"/>
     </row>
-    <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="123" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="23" t="s">
         <v>305</v>
       </c>
@@ -5113,23 +5128,25 @@
       <c r="E123" s="71" t="s">
         <v>280</v>
       </c>
-      <c r="F123" s="66"/>
+      <c r="F123" s="81" t="s">
+        <v>309</v>
+      </c>
       <c r="G123" s="66"/>
       <c r="H123" s="66"/>
       <c r="I123" s="66"/>
     </row>
     <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="23" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="B124" s="8" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="C124" s="18" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="D124" s="8" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="E124" s="71" t="s">
         <v>280</v>
@@ -5141,16 +5158,16 @@
     </row>
     <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="23" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="B125" s="8" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="C125" s="18" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="D125" s="8" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="E125" s="71" t="s">
         <v>280</v>
@@ -5162,19 +5179,19 @@
     </row>
     <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="72" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="B126" s="73" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="C126" s="18" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="D126" s="8" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="E126" s="71" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="F126" s="66"/>
       <c r="G126" s="66"/>
@@ -5183,19 +5200,19 @@
     </row>
     <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="72" t="s">
+        <v>323</v>
+      </c>
+      <c r="B127" s="73" t="s">
+        <v>324</v>
+      </c>
+      <c r="C127" s="18" t="s">
+        <v>325</v>
+      </c>
+      <c r="D127" s="8" t="s">
+        <v>326</v>
+      </c>
+      <c r="E127" s="71" t="s">
         <v>322</v>
-      </c>
-      <c r="B127" s="73" t="s">
-        <v>323</v>
-      </c>
-      <c r="C127" s="18" t="s">
-        <v>324</v>
-      </c>
-      <c r="D127" s="8" t="s">
-        <v>325</v>
-      </c>
-      <c r="E127" s="71" t="s">
-        <v>321</v>
       </c>
       <c r="F127" s="66"/>
       <c r="G127" s="66"/>
@@ -5204,19 +5221,19 @@
     </row>
     <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="72" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B128" s="73" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="C128" s="18" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="D128" s="8" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="E128" s="71" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="F128" s="66"/>
       <c r="G128" s="66"/>
@@ -5224,20 +5241,20 @@
       <c r="I128" s="66"/>
     </row>
     <row r="129" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A129" s="81" t="s">
-        <v>330</v>
+      <c r="A129" s="82" t="s">
+        <v>331</v>
       </c>
       <c r="B129" s="73" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="C129" s="18" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="D129" s="8" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="E129" s="71" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="F129" s="66"/>
       <c r="G129" s="66"/>
@@ -5246,19 +5263,19 @@
     </row>
     <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="72" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="B130" s="73" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="C130" s="18" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="D130" s="8" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="E130" s="71" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="F130" s="66"/>
       <c r="G130" s="66"/>
@@ -5267,14 +5284,14 @@
     </row>
     <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="72" t="s">
-        <v>338</v>
-      </c>
-      <c r="B131" s="82" t="s">
         <v>339</v>
+      </c>
+      <c r="B131" s="83" t="s">
+        <v>340</v>
       </c>
       <c r="C131" s="18"/>
       <c r="D131" s="8" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="E131" s="71"/>
       <c r="F131" s="66"/>
@@ -5283,11 +5300,11 @@
       <c r="I131" s="66"/>
     </row>
     <row r="132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A132" s="83" t="s">
-        <v>341</v>
-      </c>
-      <c r="B132" s="84" t="s">
+      <c r="A132" s="84" t="s">
         <v>342</v>
+      </c>
+      <c r="B132" s="85" t="s">
+        <v>343</v>
       </c>
       <c r="C132" s="66"/>
       <c r="D132" s="66"/>
@@ -5298,11 +5315,11 @@
       <c r="I132" s="66"/>
     </row>
     <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A133" s="83" t="s">
-        <v>343</v>
-      </c>
-      <c r="B133" s="84" t="s">
+      <c r="A133" s="84" t="s">
         <v>344</v>
+      </c>
+      <c r="B133" s="85" t="s">
+        <v>345</v>
       </c>
       <c r="C133" s="66"/>
       <c r="D133" s="66"/>
@@ -5313,11 +5330,11 @@
       <c r="I133" s="66"/>
     </row>
     <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A134" s="83" t="s">
-        <v>345</v>
-      </c>
-      <c r="B134" s="84" t="s">
+      <c r="A134" s="84" t="s">
         <v>346</v>
+      </c>
+      <c r="B134" s="85" t="s">
+        <v>347</v>
       </c>
       <c r="C134" s="66"/>
       <c r="D134" s="66"/>
@@ -5328,11 +5345,11 @@
       <c r="I134" s="66"/>
     </row>
     <row r="135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A135" s="83" t="s">
-        <v>347</v>
-      </c>
-      <c r="B135" s="84" t="s">
+      <c r="A135" s="84" t="s">
         <v>348</v>
+      </c>
+      <c r="B135" s="85" t="s">
+        <v>349</v>
       </c>
       <c r="C135" s="66"/>
       <c r="D135" s="66"/>
@@ -5343,11 +5360,11 @@
       <c r="I135" s="66"/>
     </row>
     <row r="136" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A136" s="83" t="s">
-        <v>349</v>
-      </c>
-      <c r="B136" s="84" t="s">
+      <c r="A136" s="84" t="s">
         <v>350</v>
+      </c>
+      <c r="B136" s="85" t="s">
+        <v>351</v>
       </c>
       <c r="C136" s="66"/>
       <c r="D136" s="66"/>
@@ -5358,11 +5375,11 @@
       <c r="I136" s="66"/>
     </row>
     <row r="137" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A137" s="83" t="s">
-        <v>351</v>
-      </c>
-      <c r="B137" s="84" t="s">
+      <c r="A137" s="84" t="s">
         <v>352</v>
+      </c>
+      <c r="B137" s="85" t="s">
+        <v>353</v>
       </c>
       <c r="C137" s="66"/>
       <c r="D137" s="66"/>
@@ -5426,8 +5443,8 @@
     </row>
     <row r="143" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="66"/>
-      <c r="B143" s="85" t="s">
-        <v>353</v>
+      <c r="B143" s="86" t="s">
+        <v>354</v>
       </c>
       <c r="C143" s="66"/>
       <c r="D143" s="66"/>
@@ -5438,15 +5455,15 @@
       <c r="I143" s="66"/>
     </row>
     <row r="144" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A144" s="86"/>
-      <c r="B144" s="87" t="s">
-        <v>354</v>
-      </c>
-      <c r="C144" s="87" t="s">
+      <c r="A144" s="87"/>
+      <c r="B144" s="88" t="s">
         <v>355</v>
       </c>
-      <c r="D144" s="88" t="s">
+      <c r="C144" s="88" t="s">
         <v>356</v>
+      </c>
+      <c r="D144" s="89" t="s">
+        <v>357</v>
       </c>
       <c r="E144" s="8" t="s">
         <v>7</v>
@@ -5459,7 +5476,7 @@
       <c r="I144" s="66"/>
     </row>
     <row r="145" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A145" s="89"/>
+      <c r="A145" s="90"/>
       <c r="B145" s="66"/>
       <c r="C145" s="66"/>
       <c r="D145" s="66"/>
@@ -5470,64 +5487,64 @@
       <c r="I145" s="66"/>
     </row>
     <row r="146" customFormat="false" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A146" s="90" t="s">
-        <v>357</v>
-      </c>
-      <c r="B146" s="91" t="s">
+      <c r="A146" s="91" t="s">
         <v>358</v>
       </c>
-      <c r="C146" s="92" t="s">
+      <c r="B146" s="92" t="s">
         <v>359</v>
       </c>
-      <c r="D146" s="93" t="s">
+      <c r="C146" s="93" t="s">
         <v>360</v>
       </c>
-      <c r="E146" s="94" t="s">
+      <c r="D146" s="94" t="s">
         <v>361</v>
       </c>
-      <c r="F146" s="95" t="s">
+      <c r="E146" s="95" t="s">
         <v>362</v>
+      </c>
+      <c r="F146" s="96" t="s">
+        <v>363</v>
       </c>
       <c r="G146" s="66"/>
       <c r="H146" s="66"/>
       <c r="I146" s="66"/>
     </row>
     <row r="147" customFormat="false" ht="85.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A147" s="90"/>
-      <c r="B147" s="96" t="s">
-        <v>363</v>
-      </c>
-      <c r="C147" s="97" t="s">
+      <c r="A147" s="91"/>
+      <c r="B147" s="97" t="s">
         <v>364</v>
       </c>
-      <c r="D147" s="98" t="s">
+      <c r="C147" s="98" t="s">
         <v>365</v>
       </c>
-      <c r="E147" s="99" t="s">
+      <c r="D147" s="99" t="s">
         <v>366</v>
       </c>
-      <c r="F147" s="95" t="s">
+      <c r="E147" s="100" t="s">
         <v>367</v>
+      </c>
+      <c r="F147" s="96" t="s">
+        <v>368</v>
       </c>
       <c r="G147" s="66"/>
       <c r="H147" s="66"/>
       <c r="I147" s="66"/>
     </row>
     <row r="148" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A148" s="90"/>
-      <c r="B148" s="100" t="s">
-        <v>368</v>
-      </c>
-      <c r="C148" s="101" t="s">
+      <c r="A148" s="91"/>
+      <c r="B148" s="101" t="s">
         <v>369</v>
       </c>
-      <c r="D148" s="102" t="s">
+      <c r="C148" s="102" t="s">
         <v>370</v>
       </c>
-      <c r="E148" s="103" t="s">
+      <c r="D148" s="103" t="s">
+        <v>371</v>
+      </c>
+      <c r="E148" s="104" t="s">
         <v>12</v>
       </c>
-      <c r="F148" s="104" t="s">
+      <c r="F148" s="105" t="s">
         <v>12</v>
       </c>
       <c r="G148" s="66"/>
@@ -5538,20 +5555,20 @@
       <c r="L148" s="66"/>
     </row>
     <row r="149" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A149" s="90"/>
-      <c r="B149" s="105" t="s">
-        <v>371</v>
-      </c>
-      <c r="C149" s="101" t="s">
-        <v>369</v>
-      </c>
-      <c r="D149" s="102" t="s">
+      <c r="A149" s="91"/>
+      <c r="B149" s="106" t="s">
         <v>372</v>
       </c>
-      <c r="E149" s="103" t="s">
+      <c r="C149" s="102" t="s">
+        <v>370</v>
+      </c>
+      <c r="D149" s="103" t="s">
+        <v>373</v>
+      </c>
+      <c r="E149" s="104" t="s">
         <v>12</v>
       </c>
-      <c r="F149" s="104" t="s">
+      <c r="F149" s="105" t="s">
         <v>12</v>
       </c>
       <c r="G149" s="66"/>
@@ -5562,20 +5579,20 @@
       <c r="L149" s="66"/>
     </row>
     <row r="150" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A150" s="90"/>
-      <c r="B150" s="106" t="s">
+      <c r="A150" s="91"/>
+      <c r="B150" s="107" t="s">
         <v>304</v>
       </c>
-      <c r="C150" s="107" t="s">
-        <v>369</v>
-      </c>
-      <c r="D150" s="108" t="s">
-        <v>373</v>
-      </c>
-      <c r="E150" s="109" t="s">
+      <c r="C150" s="108" t="s">
+        <v>370</v>
+      </c>
+      <c r="D150" s="109" t="s">
+        <v>374</v>
+      </c>
+      <c r="E150" s="110" t="s">
         <v>12</v>
       </c>
-      <c r="F150" s="110" t="s">
+      <c r="F150" s="111" t="s">
         <v>12</v>
       </c>
       <c r="G150" s="66"/>

</xml_diff>

<commit_message>
subscribe to action message
</commit_message>
<xml_diff>
--- a/documentation/Tabla_de_registros_HMI_Ivan.xlsx
+++ b/documentation/Tabla_de_registros_HMI_Ivan.xlsx
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="375">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="680" uniqueCount="376">
   <si>
     <t xml:space="preserve">Elemento IOLink</t>
   </si>
@@ -498,6 +498,9 @@
   </si>
   <si>
     <t xml:space="preserve">Registro Modbus necesario en Rasberry-Pi Para programación HMI </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Action= 14</t>
   </si>
   <si>
     <t xml:space="preserve">Función </t>
@@ -1442,7 +1445,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1477,6 +1480,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFD7"/>
         <bgColor rgb="FFFFF5CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB4C7DC"/>
+        <bgColor rgb="FFCCCCFF"/>
       </patternFill>
     </fill>
     <fill>
@@ -1748,7 +1757,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="112">
+  <cellXfs count="115">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2025,6 +2034,10 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2037,14 +2050,22 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="8" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="7" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2053,19 +2074,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="8" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="8" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="8" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="7" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="7" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="7" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2073,23 +2094,23 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="7" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="8" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="10" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2224,7 +2245,7 @@
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FFB4C7DC"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
@@ -2283,7 +2304,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="F127:F129 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2313,8 +2334,8 @@
   </sheetPr>
   <dimension ref="A1:L309"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A110" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F129" activeCellId="0" sqref="F127:F129"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A62" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H74" activeCellId="0" sqref="H74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.4453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4085,13 +4106,15 @@
       <c r="D73" s="68"/>
       <c r="E73" s="68"/>
       <c r="F73" s="66"/>
-      <c r="G73" s="66"/>
-      <c r="H73" s="66"/>
+      <c r="G73" s="69"/>
+      <c r="H73" s="66" t="s">
+        <v>100</v>
+      </c>
       <c r="I73" s="66"/>
     </row>
     <row r="74" customFormat="false" ht="46.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="23" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B74" s="8" t="s">
         <v>7</v>
@@ -4099,11 +4122,11 @@
       <c r="C74" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="D74" s="69" t="s">
-        <v>101</v>
-      </c>
-      <c r="E74" s="70" t="s">
+      <c r="D74" s="70" t="s">
         <v>102</v>
+      </c>
+      <c r="E74" s="71" t="s">
+        <v>103</v>
       </c>
       <c r="F74" s="66"/>
       <c r="H74" s="66"/>
@@ -4111,22 +4134,22 @@
     </row>
     <row r="75" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="23" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B75" s="8" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C75" s="18" t="s">
-        <v>105</v>
-      </c>
-      <c r="D75" s="71" t="s">
         <v>106</v>
       </c>
-      <c r="E75" s="71" t="s">
+      <c r="D75" s="72" t="s">
         <v>107</v>
       </c>
+      <c r="E75" s="72" t="s">
+        <v>108</v>
+      </c>
       <c r="F75" s="29" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="G75" s="29"/>
       <c r="H75" s="29"/>
@@ -4135,22 +4158,22 @@
     </row>
     <row r="76" customFormat="false" ht="43.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="23" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B76" s="8" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C76" s="18" t="s">
-        <v>111</v>
-      </c>
-      <c r="D76" s="71" t="s">
         <v>112</v>
       </c>
-      <c r="E76" s="71" t="s">
-        <v>107</v>
+      <c r="D76" s="72" t="s">
+        <v>113</v>
+      </c>
+      <c r="E76" s="72" t="s">
+        <v>108</v>
       </c>
       <c r="F76" s="29" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="G76" s="29"/>
       <c r="H76" s="29"/>
@@ -4158,146 +4181,146 @@
       <c r="J76" s="29"/>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="72" t="s">
-        <v>114</v>
-      </c>
-      <c r="B77" s="73" t="s">
+      <c r="A77" s="73" t="s">
         <v>115</v>
       </c>
+      <c r="B77" s="74" t="s">
+        <v>116</v>
+      </c>
       <c r="C77" s="18" t="s">
-        <v>116</v>
-      </c>
-      <c r="D77" s="71" t="s">
         <v>117</v>
       </c>
-      <c r="E77" s="71" t="s">
-        <v>107</v>
+      <c r="D77" s="72" t="s">
+        <v>118</v>
+      </c>
+      <c r="E77" s="72" t="s">
+        <v>108</v>
       </c>
       <c r="F77" s="66"/>
     </row>
     <row r="78" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="72" t="s">
-        <v>118</v>
-      </c>
-      <c r="B78" s="73" t="s">
+      <c r="A78" s="73" t="s">
         <v>119</v>
       </c>
+      <c r="B78" s="74" t="s">
+        <v>120</v>
+      </c>
       <c r="C78" s="18" t="s">
-        <v>120</v>
-      </c>
-      <c r="D78" s="71" t="s">
         <v>121</v>
       </c>
-      <c r="E78" s="71" t="s">
-        <v>107</v>
+      <c r="D78" s="72" t="s">
+        <v>122</v>
+      </c>
+      <c r="E78" s="72" t="s">
+        <v>108</v>
       </c>
       <c r="F78" s="66"/>
     </row>
     <row r="79" customFormat="false" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A79" s="28" t="s">
-        <v>122</v>
+      <c r="A79" s="75" t="s">
+        <v>123</v>
       </c>
       <c r="B79" s="8" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C79" s="18" t="s">
-        <v>124</v>
-      </c>
-      <c r="D79" s="71" t="s">
         <v>125</v>
       </c>
-      <c r="E79" s="71" t="s">
-        <v>107</v>
+      <c r="D79" s="72" t="s">
+        <v>126</v>
+      </c>
+      <c r="E79" s="72" t="s">
+        <v>108</v>
       </c>
       <c r="F79" s="66"/>
     </row>
     <row r="80" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A80" s="23" t="s">
-        <v>126</v>
+      <c r="A80" s="76" t="s">
+        <v>127</v>
       </c>
       <c r="B80" s="8" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C80" s="18" t="s">
-        <v>128</v>
-      </c>
-      <c r="D80" s="71" t="s">
         <v>129</v>
       </c>
-      <c r="E80" s="71" t="s">
-        <v>107</v>
+      <c r="D80" s="72" t="s">
+        <v>130</v>
+      </c>
+      <c r="E80" s="72" t="s">
+        <v>108</v>
       </c>
       <c r="F80" s="66"/>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="23" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B81" s="8" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C81" s="18" t="s">
-        <v>132</v>
-      </c>
-      <c r="D81" s="71" t="s">
         <v>133</v>
       </c>
-      <c r="E81" s="71" t="s">
-        <v>107</v>
+      <c r="D81" s="72" t="s">
+        <v>134</v>
+      </c>
+      <c r="E81" s="72" t="s">
+        <v>108</v>
       </c>
       <c r="F81" s="66"/>
     </row>
     <row r="82" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="23" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B82" s="8" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C82" s="18" t="s">
-        <v>136</v>
-      </c>
-      <c r="D82" s="71" t="s">
         <v>137</v>
       </c>
-      <c r="E82" s="71" t="s">
+      <c r="D82" s="72" t="s">
         <v>138</v>
+      </c>
+      <c r="E82" s="72" t="s">
+        <v>139</v>
       </c>
       <c r="F82" s="66"/>
     </row>
     <row r="83" customFormat="false" ht="39" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A83" s="23" t="s">
+        <v>140</v>
+      </c>
+      <c r="B83" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="C83" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="D83" s="72" t="s">
+        <v>143</v>
+      </c>
+      <c r="E83" s="72" t="s">
         <v>139</v>
-      </c>
-      <c r="B83" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="C83" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="D83" s="71" t="s">
-        <v>142</v>
-      </c>
-      <c r="E83" s="71" t="s">
-        <v>138</v>
       </c>
       <c r="F83" s="66"/>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="23" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B84" s="8" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C84" s="18" t="s">
-        <v>145</v>
-      </c>
-      <c r="D84" s="71" t="s">
         <v>146</v>
       </c>
-      <c r="E84" s="71" t="s">
-        <v>138</v>
+      <c r="D84" s="72" t="s">
+        <v>147</v>
+      </c>
+      <c r="E84" s="72" t="s">
+        <v>139</v>
       </c>
       <c r="F84" s="66"/>
       <c r="G84" s="66"/>
@@ -4306,19 +4329,19 @@
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="23" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B85" s="8" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C85" s="18" t="s">
-        <v>149</v>
-      </c>
-      <c r="D85" s="71" t="s">
         <v>150</v>
       </c>
-      <c r="E85" s="71" t="s">
-        <v>138</v>
+      <c r="D85" s="72" t="s">
+        <v>151</v>
+      </c>
+      <c r="E85" s="72" t="s">
+        <v>139</v>
       </c>
       <c r="F85" s="66"/>
       <c r="G85" s="66"/>
@@ -4327,22 +4350,22 @@
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A86" s="23" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B86" s="8" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C86" s="18" t="s">
-        <v>153</v>
-      </c>
-      <c r="D86" s="71" t="s">
         <v>154</v>
       </c>
-      <c r="E86" s="71" t="s">
-        <v>138</v>
+      <c r="D86" s="72" t="s">
+        <v>155</v>
+      </c>
+      <c r="E86" s="72" t="s">
+        <v>139</v>
       </c>
       <c r="F86" s="29" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="G86" s="29"/>
       <c r="H86" s="29"/>
@@ -4351,42 +4374,42 @@
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="23" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B87" s="8" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C87" s="18" t="s">
-        <v>158</v>
-      </c>
-      <c r="D87" s="71" t="s">
         <v>159</v>
       </c>
-      <c r="E87" s="71" t="s">
-        <v>138</v>
+      <c r="D87" s="72" t="s">
+        <v>160</v>
+      </c>
+      <c r="E87" s="72" t="s">
+        <v>139</v>
       </c>
       <c r="F87" s="66"/>
       <c r="G87" s="66"/>
       <c r="I87" s="66"/>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="72" t="s">
-        <v>160</v>
-      </c>
-      <c r="B88" s="73" t="s">
+      <c r="A88" s="73" t="s">
         <v>161</v>
       </c>
+      <c r="B88" s="74" t="s">
+        <v>162</v>
+      </c>
       <c r="C88" s="18" t="s">
-        <v>162</v>
-      </c>
-      <c r="D88" s="74" t="s">
         <v>163</v>
       </c>
-      <c r="E88" s="71" t="s">
-        <v>138</v>
+      <c r="D88" s="77" t="s">
+        <v>164</v>
+      </c>
+      <c r="E88" s="72" t="s">
+        <v>139</v>
       </c>
       <c r="F88" s="13" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="G88" s="13"/>
       <c r="H88" s="13"/>
@@ -4395,19 +4418,19 @@
     </row>
     <row r="89" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="23" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B89" s="8" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C89" s="18" t="s">
-        <v>167</v>
-      </c>
-      <c r="D89" s="71" t="s">
         <v>168</v>
       </c>
-      <c r="E89" s="71" t="s">
-        <v>107</v>
+      <c r="D89" s="72" t="s">
+        <v>169</v>
+      </c>
+      <c r="E89" s="72" t="s">
+        <v>108</v>
       </c>
       <c r="F89" s="66"/>
       <c r="G89" s="66"/>
@@ -4416,22 +4439,22 @@
     </row>
     <row r="90" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A90" s="23" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B90" s="8" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C90" s="18" t="s">
-        <v>171</v>
-      </c>
-      <c r="D90" s="71" t="s">
         <v>172</v>
       </c>
-      <c r="E90" s="71" t="s">
+      <c r="D90" s="72" t="s">
         <v>173</v>
       </c>
+      <c r="E90" s="72" t="s">
+        <v>174</v>
+      </c>
       <c r="F90" s="29" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="G90" s="29"/>
       <c r="H90" s="29"/>
@@ -4439,20 +4462,20 @@
       <c r="J90" s="29"/>
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="72" t="s">
-        <v>175</v>
-      </c>
-      <c r="B91" s="73" t="s">
+      <c r="A91" s="73" t="s">
         <v>176</v>
       </c>
+      <c r="B91" s="74" t="s">
+        <v>177</v>
+      </c>
       <c r="C91" s="18" t="s">
-        <v>177</v>
-      </c>
-      <c r="D91" s="75" t="s">
         <v>178</v>
       </c>
-      <c r="E91" s="71" t="s">
+      <c r="D91" s="78" t="s">
         <v>179</v>
+      </c>
+      <c r="E91" s="72" t="s">
+        <v>180</v>
       </c>
       <c r="F91" s="66"/>
       <c r="G91" s="66"/>
@@ -4460,20 +4483,20 @@
       <c r="I91" s="66"/>
     </row>
     <row r="92" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="72" t="s">
-        <v>118</v>
-      </c>
-      <c r="B92" s="73" t="s">
+      <c r="A92" s="73" t="s">
+        <v>119</v>
+      </c>
+      <c r="B92" s="74" t="s">
+        <v>181</v>
+      </c>
+      <c r="C92" s="18" t="s">
+        <v>182</v>
+      </c>
+      <c r="D92" s="72" t="s">
+        <v>183</v>
+      </c>
+      <c r="E92" s="72" t="s">
         <v>180</v>
-      </c>
-      <c r="C92" s="18" t="s">
-        <v>181</v>
-      </c>
-      <c r="D92" s="71" t="s">
-        <v>182</v>
-      </c>
-      <c r="E92" s="71" t="s">
-        <v>179</v>
       </c>
       <c r="F92" s="66"/>
       <c r="G92" s="66"/>
@@ -4481,20 +4504,20 @@
       <c r="I92" s="66"/>
     </row>
     <row r="93" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="76" t="s">
-        <v>183</v>
-      </c>
-      <c r="B93" s="73" t="s">
+      <c r="A93" s="79" t="s">
         <v>184</v>
       </c>
+      <c r="B93" s="74" t="s">
+        <v>185</v>
+      </c>
       <c r="C93" s="18" t="s">
-        <v>185</v>
-      </c>
-      <c r="D93" s="71" t="s">
         <v>186</v>
       </c>
-      <c r="E93" s="71" t="s">
-        <v>179</v>
+      <c r="D93" s="72" t="s">
+        <v>187</v>
+      </c>
+      <c r="E93" s="72" t="s">
+        <v>180</v>
       </c>
       <c r="F93" s="66"/>
       <c r="G93" s="66"/>
@@ -4502,20 +4525,20 @@
       <c r="I93" s="66"/>
     </row>
     <row r="94" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="77" t="s">
-        <v>187</v>
-      </c>
-      <c r="B94" s="73" t="s">
+      <c r="A94" s="80" t="s">
         <v>188</v>
       </c>
+      <c r="B94" s="74" t="s">
+        <v>189</v>
+      </c>
       <c r="C94" s="18" t="s">
-        <v>189</v>
-      </c>
-      <c r="D94" s="71" t="s">
         <v>190</v>
       </c>
-      <c r="E94" s="71" t="s">
-        <v>179</v>
+      <c r="D94" s="72" t="s">
+        <v>191</v>
+      </c>
+      <c r="E94" s="72" t="s">
+        <v>180</v>
       </c>
       <c r="F94" s="66"/>
       <c r="G94" s="66"/>
@@ -4523,20 +4546,20 @@
       <c r="I94" s="66"/>
     </row>
     <row r="95" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="23" t="s">
-        <v>191</v>
+      <c r="A95" s="76" t="s">
+        <v>192</v>
       </c>
       <c r="B95" s="8" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C95" s="18" t="s">
-        <v>193</v>
-      </c>
-      <c r="D95" s="71" t="s">
         <v>194</v>
       </c>
-      <c r="E95" s="71" t="s">
-        <v>179</v>
+      <c r="D95" s="72" t="s">
+        <v>195</v>
+      </c>
+      <c r="E95" s="72" t="s">
+        <v>180</v>
       </c>
       <c r="F95" s="66"/>
       <c r="G95" s="66"/>
@@ -4544,20 +4567,20 @@
       <c r="I95" s="66"/>
     </row>
     <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="23" t="s">
-        <v>195</v>
+      <c r="A96" s="76" t="s">
+        <v>196</v>
       </c>
       <c r="B96" s="8" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C96" s="18" t="s">
-        <v>197</v>
-      </c>
-      <c r="D96" s="71" t="s">
         <v>198</v>
       </c>
-      <c r="E96" s="71" t="s">
-        <v>179</v>
+      <c r="D96" s="72" t="s">
+        <v>199</v>
+      </c>
+      <c r="E96" s="72" t="s">
+        <v>180</v>
       </c>
       <c r="F96" s="66"/>
       <c r="G96" s="66"/>
@@ -4565,20 +4588,20 @@
       <c r="I96" s="66"/>
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="23" t="s">
-        <v>199</v>
+      <c r="A97" s="76" t="s">
+        <v>200</v>
       </c>
       <c r="B97" s="8" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C97" s="18" t="s">
-        <v>201</v>
-      </c>
-      <c r="D97" s="71" t="s">
         <v>202</v>
       </c>
-      <c r="E97" s="71" t="s">
-        <v>179</v>
+      <c r="D97" s="72" t="s">
+        <v>203</v>
+      </c>
+      <c r="E97" s="72" t="s">
+        <v>180</v>
       </c>
       <c r="F97" s="66"/>
       <c r="G97" s="66"/>
@@ -4586,20 +4609,20 @@
       <c r="I97" s="66"/>
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="23" t="s">
-        <v>203</v>
+      <c r="A98" s="76" t="s">
+        <v>204</v>
       </c>
       <c r="B98" s="8" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C98" s="18" t="s">
-        <v>205</v>
-      </c>
-      <c r="D98" s="74" t="s">
         <v>206</v>
       </c>
-      <c r="E98" s="71" t="s">
-        <v>179</v>
+      <c r="D98" s="77" t="s">
+        <v>207</v>
+      </c>
+      <c r="E98" s="72" t="s">
+        <v>180</v>
       </c>
       <c r="F98" s="66"/>
       <c r="G98" s="66"/>
@@ -4607,20 +4630,20 @@
       <c r="I98" s="66"/>
     </row>
     <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="23" t="s">
-        <v>207</v>
+      <c r="A99" s="76" t="s">
+        <v>208</v>
       </c>
       <c r="B99" s="8" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C99" s="18" t="s">
-        <v>209</v>
-      </c>
-      <c r="D99" s="71" t="s">
         <v>210</v>
       </c>
-      <c r="E99" s="71" t="s">
-        <v>179</v>
+      <c r="D99" s="72" t="s">
+        <v>211</v>
+      </c>
+      <c r="E99" s="72" t="s">
+        <v>180</v>
       </c>
       <c r="F99" s="66"/>
       <c r="G99" s="66"/>
@@ -4629,22 +4652,22 @@
     </row>
     <row r="100" customFormat="false" ht="26.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A100" s="23" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B100" s="8" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C100" s="18" t="s">
-        <v>212</v>
-      </c>
-      <c r="D100" s="71" t="s">
         <v>213</v>
       </c>
-      <c r="E100" s="71" t="s">
-        <v>179</v>
+      <c r="D100" s="72" t="s">
+        <v>214</v>
+      </c>
+      <c r="E100" s="72" t="s">
+        <v>180</v>
       </c>
       <c r="F100" s="29" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="G100" s="29"/>
       <c r="H100" s="29"/>
@@ -4653,19 +4676,19 @@
     </row>
     <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="23" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B101" s="8" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C101" s="18" t="s">
-        <v>216</v>
-      </c>
-      <c r="D101" s="71" t="s">
         <v>217</v>
       </c>
-      <c r="E101" s="71" t="s">
-        <v>179</v>
+      <c r="D101" s="72" t="s">
+        <v>218</v>
+      </c>
+      <c r="E101" s="72" t="s">
+        <v>180</v>
       </c>
       <c r="F101" s="66"/>
       <c r="G101" s="66"/>
@@ -4674,19 +4697,19 @@
     </row>
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="23" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B102" s="8" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C102" s="18" t="s">
-        <v>220</v>
-      </c>
-      <c r="D102" s="71" t="s">
         <v>221</v>
       </c>
-      <c r="E102" s="71" t="s">
-        <v>179</v>
+      <c r="D102" s="72" t="s">
+        <v>222</v>
+      </c>
+      <c r="E102" s="72" t="s">
+        <v>180</v>
       </c>
       <c r="F102" s="66"/>
       <c r="G102" s="66"/>
@@ -4694,20 +4717,20 @@
       <c r="I102" s="66"/>
     </row>
     <row r="103" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A103" s="23" t="s">
-        <v>222</v>
+      <c r="A103" s="76" t="s">
+        <v>223</v>
       </c>
       <c r="B103" s="8" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C103" s="18" t="s">
-        <v>224</v>
-      </c>
-      <c r="D103" s="71" t="s">
         <v>225</v>
       </c>
-      <c r="E103" s="71" t="s">
+      <c r="D103" s="72" t="s">
         <v>226</v>
+      </c>
+      <c r="E103" s="72" t="s">
+        <v>227</v>
       </c>
       <c r="F103" s="66"/>
       <c r="G103" s="66"/>
@@ -4715,20 +4738,20 @@
       <c r="I103" s="66"/>
     </row>
     <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="23" t="s">
+      <c r="A104" s="76" t="s">
+        <v>228</v>
+      </c>
+      <c r="B104" s="8" t="s">
+        <v>229</v>
+      </c>
+      <c r="C104" s="18" t="s">
+        <v>230</v>
+      </c>
+      <c r="D104" s="72" t="s">
+        <v>231</v>
+      </c>
+      <c r="E104" s="72" t="s">
         <v>227</v>
-      </c>
-      <c r="B104" s="8" t="s">
-        <v>228</v>
-      </c>
-      <c r="C104" s="18" t="s">
-        <v>229</v>
-      </c>
-      <c r="D104" s="71" t="s">
-        <v>230</v>
-      </c>
-      <c r="E104" s="71" t="s">
-        <v>226</v>
       </c>
       <c r="F104" s="66"/>
       <c r="G104" s="66"/>
@@ -4737,19 +4760,19 @@
     </row>
     <row r="105" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A105" s="23" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B105" s="8" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C105" s="18" t="s">
-        <v>232</v>
-      </c>
-      <c r="D105" s="71" t="s">
-        <v>150</v>
-      </c>
-      <c r="E105" s="71" t="s">
-        <v>226</v>
+        <v>233</v>
+      </c>
+      <c r="D105" s="72" t="s">
+        <v>151</v>
+      </c>
+      <c r="E105" s="72" t="s">
+        <v>227</v>
       </c>
       <c r="F105" s="66"/>
       <c r="G105" s="66"/>
@@ -4757,23 +4780,23 @@
       <c r="I105" s="66"/>
     </row>
     <row r="106" customFormat="false" ht="74.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A106" s="78" t="s">
-        <v>233</v>
-      </c>
-      <c r="B106" s="73" t="s">
+      <c r="A106" s="81" t="s">
         <v>234</v>
       </c>
+      <c r="B106" s="74" t="s">
+        <v>235</v>
+      </c>
       <c r="C106" s="18" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="D106" s="8" t="s">
-        <v>236</v>
-      </c>
-      <c r="E106" s="71" t="s">
         <v>237</v>
       </c>
+      <c r="E106" s="72" t="s">
+        <v>238</v>
+      </c>
       <c r="F106" s="8" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="G106" s="8"/>
       <c r="H106" s="8"/>
@@ -4781,74 +4804,74 @@
       <c r="J106" s="8"/>
     </row>
     <row r="107" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="76" t="s">
-        <v>239</v>
-      </c>
-      <c r="B107" s="73" t="s">
+      <c r="A107" s="79" t="s">
         <v>240</v>
       </c>
+      <c r="B107" s="74" t="s">
+        <v>241</v>
+      </c>
       <c r="C107" s="18" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="D107" s="8" t="s">
-        <v>242</v>
-      </c>
-      <c r="E107" s="71" t="s">
-        <v>237</v>
+        <v>243</v>
+      </c>
+      <c r="E107" s="72" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A108" s="72" t="s">
-        <v>243</v>
-      </c>
-      <c r="B108" s="73" t="s">
+      <c r="A108" s="73" t="s">
         <v>244</v>
       </c>
+      <c r="B108" s="74" t="s">
+        <v>245</v>
+      </c>
       <c r="C108" s="18" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="D108" s="8" t="s">
-        <v>246</v>
-      </c>
-      <c r="E108" s="71" t="s">
-        <v>237</v>
+        <v>247</v>
+      </c>
+      <c r="E108" s="72" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A109" s="72" t="s">
-        <v>247</v>
-      </c>
-      <c r="B109" s="73" t="s">
+      <c r="A109" s="73" t="s">
         <v>248</v>
       </c>
+      <c r="B109" s="74" t="s">
+        <v>249</v>
+      </c>
       <c r="C109" s="18" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="D109" s="8" t="s">
-        <v>250</v>
-      </c>
-      <c r="E109" s="71" t="s">
-        <v>237</v>
+        <v>251</v>
+      </c>
+      <c r="E109" s="72" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="142.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A110" s="79" t="s">
-        <v>251</v>
+      <c r="A110" s="82" t="s">
+        <v>252</v>
       </c>
       <c r="B110" s="8" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C110" s="18" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="D110" s="8" t="s">
-        <v>254</v>
-      </c>
-      <c r="E110" s="71" t="s">
         <v>255</v>
       </c>
+      <c r="E110" s="72" t="s">
+        <v>256</v>
+      </c>
       <c r="F110" s="8" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="G110" s="8"/>
       <c r="H110" s="8"/>
@@ -4856,20 +4879,20 @@
       <c r="J110" s="8"/>
     </row>
     <row r="111" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A111" s="79" t="s">
-        <v>257</v>
+      <c r="A111" s="82" t="s">
+        <v>258</v>
       </c>
       <c r="B111" s="8" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C111" s="18" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="D111" s="8" t="s">
-        <v>260</v>
-      </c>
-      <c r="E111" s="71" t="s">
-        <v>255</v>
+        <v>261</v>
+      </c>
+      <c r="E111" s="72" t="s">
+        <v>256</v>
       </c>
       <c r="F111" s="66"/>
       <c r="G111" s="66"/>
@@ -4877,87 +4900,87 @@
       <c r="I111" s="66"/>
     </row>
     <row r="112" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A112" s="23" t="s">
-        <v>261</v>
+      <c r="A112" s="76" t="s">
+        <v>262</v>
       </c>
       <c r="B112" s="8" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="C112" s="18" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="D112" s="8" t="s">
-        <v>198</v>
-      </c>
-      <c r="E112" s="71" t="s">
-        <v>255</v>
+        <v>199</v>
+      </c>
+      <c r="E112" s="72" t="s">
+        <v>256</v>
       </c>
       <c r="F112" s="8" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="G112" s="8"/>
       <c r="H112" s="8"/>
       <c r="I112" s="8"/>
     </row>
     <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A113" s="23" t="s">
-        <v>265</v>
+      <c r="A113" s="76" t="s">
+        <v>266</v>
       </c>
       <c r="B113" s="8" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C113" s="18" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="D113" s="8" t="s">
-        <v>202</v>
-      </c>
-      <c r="E113" s="71" t="s">
-        <v>255</v>
+        <v>203</v>
+      </c>
+      <c r="E113" s="72" t="s">
+        <v>256</v>
       </c>
       <c r="G113" s="66"/>
       <c r="H113" s="66"/>
       <c r="I113" s="66"/>
     </row>
     <row r="114" customFormat="false" ht="26.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A114" s="79" t="s">
-        <v>268</v>
+      <c r="A114" s="82" t="s">
+        <v>269</v>
       </c>
       <c r="B114" s="8" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="C114" s="18" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="D114" s="21" t="s">
-        <v>271</v>
-      </c>
-      <c r="E114" s="71" t="s">
-        <v>255</v>
-      </c>
-      <c r="F114" s="80" t="s">
         <v>272</v>
       </c>
-      <c r="G114" s="80"/>
-      <c r="H114" s="80"/>
-      <c r="I114" s="80"/>
-      <c r="J114" s="80"/>
+      <c r="E114" s="72" t="s">
+        <v>256</v>
+      </c>
+      <c r="F114" s="83" t="s">
+        <v>273</v>
+      </c>
+      <c r="G114" s="83"/>
+      <c r="H114" s="83"/>
+      <c r="I114" s="83"/>
+      <c r="J114" s="83"/>
     </row>
     <row r="115" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A115" s="23" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B115" s="8" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C115" s="18" t="s">
-        <v>275</v>
-      </c>
-      <c r="D115" s="71" t="s">
-        <v>221</v>
-      </c>
-      <c r="E115" s="71" t="s">
-        <v>255</v>
+        <v>276</v>
+      </c>
+      <c r="D115" s="72" t="s">
+        <v>222</v>
+      </c>
+      <c r="E115" s="72" t="s">
+        <v>256</v>
       </c>
       <c r="F115" s="66"/>
       <c r="G115" s="66"/>
@@ -4965,20 +4988,20 @@
       <c r="I115" s="66"/>
     </row>
     <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A116" s="72" t="s">
-        <v>276</v>
-      </c>
-      <c r="B116" s="73" t="s">
+      <c r="A116" s="73" t="s">
         <v>277</v>
       </c>
+      <c r="B116" s="74" t="s">
+        <v>278</v>
+      </c>
       <c r="C116" s="18" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="D116" s="8" t="s">
-        <v>279</v>
-      </c>
-      <c r="E116" s="71" t="s">
         <v>280</v>
+      </c>
+      <c r="E116" s="72" t="s">
+        <v>281</v>
       </c>
       <c r="F116" s="66"/>
       <c r="G116" s="66"/>
@@ -4986,20 +5009,20 @@
       <c r="I116" s="66"/>
     </row>
     <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A117" s="72" t="s">
+      <c r="A117" s="73" t="s">
+        <v>282</v>
+      </c>
+      <c r="B117" s="74" t="s">
+        <v>283</v>
+      </c>
+      <c r="C117" s="18" t="s">
+        <v>284</v>
+      </c>
+      <c r="D117" s="8" t="s">
+        <v>285</v>
+      </c>
+      <c r="E117" s="72" t="s">
         <v>281</v>
-      </c>
-      <c r="B117" s="73" t="s">
-        <v>282</v>
-      </c>
-      <c r="C117" s="18" t="s">
-        <v>283</v>
-      </c>
-      <c r="D117" s="8" t="s">
-        <v>284</v>
-      </c>
-      <c r="E117" s="71" t="s">
-        <v>280</v>
       </c>
       <c r="F117" s="66"/>
       <c r="G117" s="66"/>
@@ -5007,20 +5030,20 @@
       <c r="I117" s="66"/>
     </row>
     <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A118" s="72" t="s">
-        <v>285</v>
-      </c>
-      <c r="B118" s="73" t="s">
+      <c r="A118" s="73" t="s">
         <v>286</v>
       </c>
+      <c r="B118" s="74" t="s">
+        <v>287</v>
+      </c>
       <c r="C118" s="18" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D118" s="8" t="s">
-        <v>288</v>
-      </c>
-      <c r="E118" s="71" t="s">
-        <v>280</v>
+        <v>289</v>
+      </c>
+      <c r="E118" s="72" t="s">
+        <v>281</v>
       </c>
       <c r="F118" s="66"/>
       <c r="G118" s="66"/>
@@ -5028,20 +5051,20 @@
       <c r="I118" s="66"/>
     </row>
     <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A119" s="72" t="s">
-        <v>289</v>
-      </c>
-      <c r="B119" s="73" t="s">
+      <c r="A119" s="73" t="s">
         <v>290</v>
       </c>
+      <c r="B119" s="74" t="s">
+        <v>291</v>
+      </c>
       <c r="C119" s="18" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="D119" s="8" t="s">
-        <v>292</v>
-      </c>
-      <c r="E119" s="71" t="s">
-        <v>280</v>
+        <v>293</v>
+      </c>
+      <c r="E119" s="72" t="s">
+        <v>281</v>
       </c>
       <c r="F119" s="66"/>
       <c r="G119" s="66"/>
@@ -5049,20 +5072,20 @@
       <c r="I119" s="66"/>
     </row>
     <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A120" s="72" t="s">
-        <v>293</v>
-      </c>
-      <c r="B120" s="73" t="s">
+      <c r="A120" s="73" t="s">
         <v>294</v>
       </c>
+      <c r="B120" s="74" t="s">
+        <v>295</v>
+      </c>
       <c r="C120" s="18" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="D120" s="8" t="s">
-        <v>296</v>
-      </c>
-      <c r="E120" s="71" t="s">
-        <v>280</v>
+        <v>297</v>
+      </c>
+      <c r="E120" s="72" t="s">
+        <v>281</v>
       </c>
       <c r="F120" s="8"/>
       <c r="G120" s="8"/>
@@ -5071,20 +5094,20 @@
       <c r="J120" s="8"/>
     </row>
     <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A121" s="72" t="s">
-        <v>297</v>
-      </c>
-      <c r="B121" s="73" t="s">
+      <c r="A121" s="73" t="s">
         <v>298</v>
       </c>
+      <c r="B121" s="74" t="s">
+        <v>299</v>
+      </c>
       <c r="C121" s="18" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="D121" s="8" t="s">
-        <v>300</v>
-      </c>
-      <c r="E121" s="71" t="s">
-        <v>280</v>
+        <v>301</v>
+      </c>
+      <c r="E121" s="72" t="s">
+        <v>281</v>
       </c>
       <c r="F121" s="66"/>
       <c r="G121" s="66"/>
@@ -5092,20 +5115,20 @@
       <c r="I121" s="66"/>
     </row>
     <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A122" s="72" t="s">
-        <v>301</v>
-      </c>
-      <c r="B122" s="73" t="s">
+      <c r="A122" s="73" t="s">
         <v>302</v>
       </c>
+      <c r="B122" s="74" t="s">
+        <v>303</v>
+      </c>
       <c r="C122" s="18" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="D122" s="8" t="s">
-        <v>304</v>
-      </c>
-      <c r="E122" s="71" t="s">
-        <v>280</v>
+        <v>305</v>
+      </c>
+      <c r="E122" s="72" t="s">
+        <v>281</v>
       </c>
       <c r="F122" s="66"/>
       <c r="G122" s="66"/>
@@ -5114,22 +5137,22 @@
     </row>
     <row r="123" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="23" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="B123" s="8" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="C123" s="18" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="D123" s="8" t="s">
-        <v>308</v>
-      </c>
-      <c r="E123" s="71" t="s">
-        <v>280</v>
-      </c>
-      <c r="F123" s="81" t="s">
         <v>309</v>
+      </c>
+      <c r="E123" s="72" t="s">
+        <v>281</v>
+      </c>
+      <c r="F123" s="84" t="s">
+        <v>310</v>
       </c>
       <c r="G123" s="66"/>
       <c r="H123" s="66"/>
@@ -5137,19 +5160,19 @@
     </row>
     <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="23" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="B124" s="8" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="C124" s="18" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="D124" s="8" t="s">
-        <v>313</v>
-      </c>
-      <c r="E124" s="71" t="s">
-        <v>280</v>
+        <v>314</v>
+      </c>
+      <c r="E124" s="72" t="s">
+        <v>281</v>
       </c>
       <c r="F124" s="66"/>
       <c r="G124" s="66"/>
@@ -5158,19 +5181,19 @@
     </row>
     <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="23" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="B125" s="8" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="C125" s="18" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="D125" s="8" t="s">
-        <v>317</v>
-      </c>
-      <c r="E125" s="71" t="s">
-        <v>280</v>
+        <v>318</v>
+      </c>
+      <c r="E125" s="72" t="s">
+        <v>281</v>
       </c>
       <c r="F125" s="66"/>
       <c r="G125" s="66"/>
@@ -5178,20 +5201,20 @@
       <c r="I125" s="66"/>
     </row>
     <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A126" s="72" t="s">
-        <v>318</v>
-      </c>
-      <c r="B126" s="73" t="s">
+      <c r="A126" s="73" t="s">
         <v>319</v>
       </c>
+      <c r="B126" s="74" t="s">
+        <v>320</v>
+      </c>
       <c r="C126" s="18" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="D126" s="8" t="s">
-        <v>321</v>
-      </c>
-      <c r="E126" s="71" t="s">
         <v>322</v>
+      </c>
+      <c r="E126" s="72" t="s">
+        <v>323</v>
       </c>
       <c r="F126" s="66"/>
       <c r="G126" s="66"/>
@@ -5199,20 +5222,20 @@
       <c r="I126" s="66"/>
     </row>
     <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A127" s="72" t="s">
+      <c r="A127" s="73" t="s">
+        <v>324</v>
+      </c>
+      <c r="B127" s="74" t="s">
+        <v>325</v>
+      </c>
+      <c r="C127" s="18" t="s">
+        <v>326</v>
+      </c>
+      <c r="D127" s="8" t="s">
+        <v>327</v>
+      </c>
+      <c r="E127" s="72" t="s">
         <v>323</v>
-      </c>
-      <c r="B127" s="73" t="s">
-        <v>324</v>
-      </c>
-      <c r="C127" s="18" t="s">
-        <v>325</v>
-      </c>
-      <c r="D127" s="8" t="s">
-        <v>326</v>
-      </c>
-      <c r="E127" s="71" t="s">
-        <v>322</v>
       </c>
       <c r="F127" s="66"/>
       <c r="G127" s="66"/>
@@ -5220,20 +5243,20 @@
       <c r="I127" s="66"/>
     </row>
     <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A128" s="72" t="s">
-        <v>327</v>
-      </c>
-      <c r="B128" s="73" t="s">
+      <c r="A128" s="73" t="s">
         <v>328</v>
       </c>
+      <c r="B128" s="74" t="s">
+        <v>329</v>
+      </c>
       <c r="C128" s="18" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="D128" s="8" t="s">
-        <v>330</v>
-      </c>
-      <c r="E128" s="71" t="s">
-        <v>322</v>
+        <v>331</v>
+      </c>
+      <c r="E128" s="72" t="s">
+        <v>323</v>
       </c>
       <c r="F128" s="66"/>
       <c r="G128" s="66"/>
@@ -5241,20 +5264,20 @@
       <c r="I128" s="66"/>
     </row>
     <row r="129" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A129" s="82" t="s">
-        <v>331</v>
-      </c>
-      <c r="B129" s="73" t="s">
+      <c r="A129" s="85" t="s">
         <v>332</v>
       </c>
+      <c r="B129" s="74" t="s">
+        <v>333</v>
+      </c>
       <c r="C129" s="18" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="D129" s="8" t="s">
-        <v>334</v>
-      </c>
-      <c r="E129" s="71" t="s">
-        <v>322</v>
+        <v>335</v>
+      </c>
+      <c r="E129" s="72" t="s">
+        <v>323</v>
       </c>
       <c r="F129" s="66"/>
       <c r="G129" s="66"/>
@@ -5262,20 +5285,20 @@
       <c r="I129" s="66"/>
     </row>
     <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A130" s="72" t="s">
-        <v>335</v>
-      </c>
-      <c r="B130" s="73" t="s">
+      <c r="A130" s="73" t="s">
         <v>336</v>
       </c>
+      <c r="B130" s="74" t="s">
+        <v>337</v>
+      </c>
       <c r="C130" s="18" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="D130" s="8" t="s">
-        <v>338</v>
-      </c>
-      <c r="E130" s="71" t="s">
-        <v>322</v>
+        <v>339</v>
+      </c>
+      <c r="E130" s="72" t="s">
+        <v>323</v>
       </c>
       <c r="F130" s="66"/>
       <c r="G130" s="66"/>
@@ -5283,28 +5306,28 @@
       <c r="I130" s="66"/>
     </row>
     <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A131" s="72" t="s">
-        <v>339</v>
-      </c>
-      <c r="B131" s="83" t="s">
+      <c r="A131" s="73" t="s">
         <v>340</v>
+      </c>
+      <c r="B131" s="86" t="s">
+        <v>341</v>
       </c>
       <c r="C131" s="18"/>
       <c r="D131" s="8" t="s">
-        <v>341</v>
-      </c>
-      <c r="E131" s="71"/>
+        <v>342</v>
+      </c>
+      <c r="E131" s="72"/>
       <c r="F131" s="66"/>
       <c r="G131" s="66"/>
       <c r="H131" s="66"/>
       <c r="I131" s="66"/>
     </row>
     <row r="132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A132" s="84" t="s">
-        <v>342</v>
-      </c>
-      <c r="B132" s="85" t="s">
+      <c r="A132" s="87" t="s">
         <v>343</v>
+      </c>
+      <c r="B132" s="88" t="s">
+        <v>344</v>
       </c>
       <c r="C132" s="66"/>
       <c r="D132" s="66"/>
@@ -5315,11 +5338,11 @@
       <c r="I132" s="66"/>
     </row>
     <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A133" s="84" t="s">
-        <v>344</v>
-      </c>
-      <c r="B133" s="85" t="s">
+      <c r="A133" s="87" t="s">
         <v>345</v>
+      </c>
+      <c r="B133" s="88" t="s">
+        <v>346</v>
       </c>
       <c r="C133" s="66"/>
       <c r="D133" s="66"/>
@@ -5330,11 +5353,11 @@
       <c r="I133" s="66"/>
     </row>
     <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A134" s="84" t="s">
-        <v>346</v>
-      </c>
-      <c r="B134" s="85" t="s">
+      <c r="A134" s="87" t="s">
         <v>347</v>
+      </c>
+      <c r="B134" s="88" t="s">
+        <v>348</v>
       </c>
       <c r="C134" s="66"/>
       <c r="D134" s="66"/>
@@ -5345,11 +5368,11 @@
       <c r="I134" s="66"/>
     </row>
     <row r="135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A135" s="84" t="s">
-        <v>348</v>
-      </c>
-      <c r="B135" s="85" t="s">
+      <c r="A135" s="87" t="s">
         <v>349</v>
+      </c>
+      <c r="B135" s="88" t="s">
+        <v>350</v>
       </c>
       <c r="C135" s="66"/>
       <c r="D135" s="66"/>
@@ -5360,11 +5383,11 @@
       <c r="I135" s="66"/>
     </row>
     <row r="136" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A136" s="84" t="s">
-        <v>350</v>
-      </c>
-      <c r="B136" s="85" t="s">
+      <c r="A136" s="87" t="s">
         <v>351</v>
+      </c>
+      <c r="B136" s="88" t="s">
+        <v>352</v>
       </c>
       <c r="C136" s="66"/>
       <c r="D136" s="66"/>
@@ -5375,11 +5398,11 @@
       <c r="I136" s="66"/>
     </row>
     <row r="137" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A137" s="84" t="s">
-        <v>352</v>
-      </c>
-      <c r="B137" s="85" t="s">
+      <c r="A137" s="87" t="s">
         <v>353</v>
+      </c>
+      <c r="B137" s="88" t="s">
+        <v>354</v>
       </c>
       <c r="C137" s="66"/>
       <c r="D137" s="66"/>
@@ -5443,8 +5466,8 @@
     </row>
     <row r="143" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="66"/>
-      <c r="B143" s="86" t="s">
-        <v>354</v>
+      <c r="B143" s="89" t="s">
+        <v>355</v>
       </c>
       <c r="C143" s="66"/>
       <c r="D143" s="66"/>
@@ -5455,15 +5478,15 @@
       <c r="I143" s="66"/>
     </row>
     <row r="144" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A144" s="87"/>
-      <c r="B144" s="88" t="s">
-        <v>355</v>
-      </c>
-      <c r="C144" s="88" t="s">
+      <c r="A144" s="90"/>
+      <c r="B144" s="91" t="s">
         <v>356</v>
       </c>
-      <c r="D144" s="89" t="s">
+      <c r="C144" s="91" t="s">
         <v>357</v>
+      </c>
+      <c r="D144" s="92" t="s">
+        <v>358</v>
       </c>
       <c r="E144" s="8" t="s">
         <v>7</v>
@@ -5476,7 +5499,7 @@
       <c r="I144" s="66"/>
     </row>
     <row r="145" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A145" s="90"/>
+      <c r="A145" s="93"/>
       <c r="B145" s="66"/>
       <c r="C145" s="66"/>
       <c r="D145" s="66"/>
@@ -5487,64 +5510,64 @@
       <c r="I145" s="66"/>
     </row>
     <row r="146" customFormat="false" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A146" s="91" t="s">
-        <v>358</v>
-      </c>
-      <c r="B146" s="92" t="s">
+      <c r="A146" s="94" t="s">
         <v>359</v>
       </c>
-      <c r="C146" s="93" t="s">
+      <c r="B146" s="95" t="s">
         <v>360</v>
       </c>
-      <c r="D146" s="94" t="s">
+      <c r="C146" s="96" t="s">
         <v>361</v>
       </c>
-      <c r="E146" s="95" t="s">
+      <c r="D146" s="97" t="s">
         <v>362</v>
       </c>
-      <c r="F146" s="96" t="s">
+      <c r="E146" s="98" t="s">
         <v>363</v>
+      </c>
+      <c r="F146" s="99" t="s">
+        <v>364</v>
       </c>
       <c r="G146" s="66"/>
       <c r="H146" s="66"/>
       <c r="I146" s="66"/>
     </row>
     <row r="147" customFormat="false" ht="85.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A147" s="91"/>
-      <c r="B147" s="97" t="s">
-        <v>364</v>
-      </c>
-      <c r="C147" s="98" t="s">
+      <c r="A147" s="94"/>
+      <c r="B147" s="100" t="s">
         <v>365</v>
       </c>
-      <c r="D147" s="99" t="s">
+      <c r="C147" s="101" t="s">
         <v>366</v>
       </c>
-      <c r="E147" s="100" t="s">
+      <c r="D147" s="102" t="s">
         <v>367</v>
       </c>
-      <c r="F147" s="96" t="s">
+      <c r="E147" s="103" t="s">
         <v>368</v>
+      </c>
+      <c r="F147" s="99" t="s">
+        <v>369</v>
       </c>
       <c r="G147" s="66"/>
       <c r="H147" s="66"/>
       <c r="I147" s="66"/>
     </row>
     <row r="148" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A148" s="91"/>
-      <c r="B148" s="101" t="s">
-        <v>369</v>
-      </c>
-      <c r="C148" s="102" t="s">
+      <c r="A148" s="94"/>
+      <c r="B148" s="104" t="s">
         <v>370</v>
       </c>
-      <c r="D148" s="103" t="s">
+      <c r="C148" s="105" t="s">
         <v>371</v>
       </c>
-      <c r="E148" s="104" t="s">
+      <c r="D148" s="106" t="s">
+        <v>372</v>
+      </c>
+      <c r="E148" s="107" t="s">
         <v>12</v>
       </c>
-      <c r="F148" s="105" t="s">
+      <c r="F148" s="108" t="s">
         <v>12</v>
       </c>
       <c r="G148" s="66"/>
@@ -5555,20 +5578,20 @@
       <c r="L148" s="66"/>
     </row>
     <row r="149" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A149" s="91"/>
-      <c r="B149" s="106" t="s">
-        <v>372</v>
-      </c>
-      <c r="C149" s="102" t="s">
-        <v>370</v>
-      </c>
-      <c r="D149" s="103" t="s">
+      <c r="A149" s="94"/>
+      <c r="B149" s="109" t="s">
         <v>373</v>
       </c>
-      <c r="E149" s="104" t="s">
+      <c r="C149" s="105" t="s">
+        <v>371</v>
+      </c>
+      <c r="D149" s="106" t="s">
+        <v>374</v>
+      </c>
+      <c r="E149" s="107" t="s">
         <v>12</v>
       </c>
-      <c r="F149" s="105" t="s">
+      <c r="F149" s="108" t="s">
         <v>12</v>
       </c>
       <c r="G149" s="66"/>
@@ -5579,20 +5602,20 @@
       <c r="L149" s="66"/>
     </row>
     <row r="150" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A150" s="91"/>
-      <c r="B150" s="107" t="s">
-        <v>304</v>
-      </c>
-      <c r="C150" s="108" t="s">
-        <v>370</v>
-      </c>
-      <c r="D150" s="109" t="s">
-        <v>374</v>
-      </c>
-      <c r="E150" s="110" t="s">
+      <c r="A150" s="94"/>
+      <c r="B150" s="110" t="s">
+        <v>305</v>
+      </c>
+      <c r="C150" s="111" t="s">
+        <v>371</v>
+      </c>
+      <c r="D150" s="112" t="s">
+        <v>375</v>
+      </c>
+      <c r="E150" s="113" t="s">
         <v>12</v>
       </c>
-      <c r="F150" s="111" t="s">
+      <c r="F150" s="114" t="s">
         <v>12</v>
       </c>
       <c r="G150" s="66"/>

</xml_diff>

<commit_message>
need to apply manifold
</commit_message>
<xml_diff>
--- a/documentation/Tabla_de_registros_HMI_Ivan.xlsx
+++ b/documentation/Tabla_de_registros_HMI_Ivan.xlsx
@@ -190,7 +190,28 @@
     <t xml:space="preserve">MW108</t>
   </si>
   <si>
-    <t xml:space="preserve">Manifold</t>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Manifold
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">(apply in control)</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Activar manifold</t>
@@ -2334,8 +2355,8 @@
   </sheetPr>
   <dimension ref="A1:L309"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A62" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H74" activeCellId="0" sqref="H74"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.4453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
using IntEnum instead of base model
</commit_message>
<xml_diff>
--- a/documentation/Tabla_de_registros_HMI_Ivan.xlsx
+++ b/documentation/Tabla_de_registros_HMI_Ivan.xlsx
@@ -36,6 +36,7 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">These goes to the HMI, will add the sensor reading to be displayed here, which are the values from IOLink data</t>
         </r>
@@ -195,6 +196,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Manifold
 </t>
@@ -206,6 +208,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(apply in control)</t>
     </r>
@@ -301,6 +304,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Cubeta llena entre el 100 y 80 </t>
     </r>
@@ -311,6 +315,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(Lleno</t>
     </r>
@@ -320,6 +325,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">)</t>
     </r>
@@ -334,6 +340,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Cubeta entre el 79 y 50 (</t>
     </r>
@@ -344,6 +351,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Medio-alto</t>
     </r>
@@ -353,6 +361,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">)</t>
     </r>
@@ -367,6 +376,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Cubeta entre el 49 y 30 (</t>
     </r>
@@ -377,6 +387,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Medio</t>
     </r>
@@ -386,6 +397,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">)</t>
     </r>
@@ -400,6 +412,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Cubeta entre el 20 y 10 (</t>
     </r>
@@ -410,6 +423,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Prevacio</t>
     </r>
@@ -419,6 +433,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">)</t>
     </r>
@@ -433,6 +448,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Cubeta entre el 5 hacia abajo (2cm) (</t>
     </r>
@@ -443,6 +459,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Vacio</t>
     </r>
@@ -452,6 +469,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">)</t>
     </r>
@@ -1370,6 +1388,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">How to know this condition??
 </t>
@@ -1381,6 +1400,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Se quiere activar
 el recirculado?</t>
@@ -1401,6 +1421,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1422,6 +1443,7 @@
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -1429,12 +1451,14 @@
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF1C1C1C"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <u val="single"/>
@@ -1442,6 +1466,7 @@
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -1449,12 +1474,14 @@
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -1462,6 +1489,7 @@
       <color rgb="FFC9211E"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -1469,11 +1497,13 @@
       <color rgb="FFFFFFFF"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="12">
@@ -2360,7 +2390,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.57"/>
@@ -2386,8 +2416,8 @@
   </sheetPr>
   <dimension ref="A1:L309"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A109" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F121" activeCellId="0" sqref="F121"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A106" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D139" activeCellId="0" sqref="D139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2395,12 +2425,12 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="26.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="61.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="45.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="45.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="34.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="18.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="13.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="20.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="20.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="24.14"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="11" style="1" width="11.43"/>
   </cols>

</xml_diff>

<commit_message>
continue logic for recycle
</commit_message>
<xml_diff>
--- a/documentation/Tabla_de_registros_HMI_Ivan.xlsx
+++ b/documentation/Tabla_de_registros_HMI_Ivan.xlsx
@@ -29,7 +29,7 @@
     <author> </author>
   </authors>
   <commentList>
-    <comment ref="B132" authorId="0">
+    <comment ref="B133" authorId="0">
       <text>
         <r>
           <rPr>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="689" uniqueCount="386">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="389">
   <si>
     <t xml:space="preserve">Elemento IOLink</t>
   </si>
@@ -1265,47 +1265,57 @@
     <t xml:space="preserve">seleccio de tamaño de cubeta (1, 2, 3)</t>
   </si>
   <si>
+    <t xml:space="preserve">bares de presion limite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HR-0022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NEW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sensor_manual_recycle_count</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HEX --------DEC
+HR-0023 – HR-40035</t>
+  </si>
+  <si>
     <t xml:space="preserve">sensor_material_pressure </t>
   </si>
   <si>
-    <t xml:space="preserve">HEX --------DEC
-HR-0022 – HR-40034</t>
+    <t xml:space="preserve">
+HR-0024 – HR-40036</t>
   </si>
   <si>
     <t xml:space="preserve">sensor_material_temperature </t>
   </si>
   <si>
-    <t xml:space="preserve">HR-0023 – HR-40035</t>
+    <t xml:space="preserve">HR-0025 – HR-40037</t>
   </si>
   <si>
     <t xml:space="preserve">sensor_laser_distance </t>
   </si>
   <si>
-    <t xml:space="preserve">HR-0024 -HR-40036</t>
+    <t xml:space="preserve">HR-0026 -HR-40038</t>
   </si>
   <si>
     <t xml:space="preserve">sensor_pressure_regulator_read_set </t>
   </si>
   <si>
-    <t xml:space="preserve">HR-0025 – HR-40037</t>
+    <t xml:space="preserve">HR-0027 – HR-40039</t>
   </si>
   <si>
     <t xml:space="preserve">sensor_pressure_regulator_read_real </t>
   </si>
   <si>
-    <t xml:space="preserve">HR-0026 – HR-40038</t>
+    <t xml:space="preserve">HR-0028 – HR-40040</t>
   </si>
   <si>
     <t xml:space="preserve">sensor_pressure_regulator_valve_read_state </t>
   </si>
   <si>
-    <t xml:space="preserve">HR-0027 – HR-40039</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sensor_manual_recycle_count</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HH-0028 – HR-40040</t>
+    <t xml:space="preserve">HR-0029 – HR-40041</t>
   </si>
   <si>
     <t xml:space="preserve">These are HMI registers</t>
@@ -1448,7 +1458,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="&quot; $&quot;* #,##0.00\ ;&quot;-$&quot;* #,##0.00\ ;&quot; $&quot;* \-#\ ;\ @\ "/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1508,6 +1518,20 @@
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="12"/>
+      <color rgb="FF1E6A39"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1865,7 +1889,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="119">
+  <cellXfs count="121">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2226,7 +2250,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2234,7 +2262,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2338,7 +2370,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2364,7 +2396,7 @@
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF1E6A39"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
@@ -2455,10 +2487,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L309"/>
+  <dimension ref="A1:L311"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A122" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B138" activeCellId="0" sqref="B138"/>
+      <selection pane="topLeft" activeCell="C141" activeCellId="0" sqref="C141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5450,42 +5482,44 @@
       <c r="H131" s="68"/>
       <c r="I131" s="68"/>
     </row>
-    <row r="132" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A132" s="90" t="s">
+    <row r="132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A132" s="75" t="s">
         <v>346</v>
       </c>
-      <c r="B132" s="91" t="s">
+      <c r="B132" s="76" t="s">
         <v>347</v>
       </c>
-      <c r="C132" s="68"/>
-      <c r="D132" s="68"/>
-      <c r="E132" s="68"/>
+      <c r="C132" s="18"/>
+      <c r="D132" s="8"/>
+      <c r="E132" s="90" t="s">
+        <v>348</v>
+      </c>
       <c r="F132" s="68"/>
       <c r="G132" s="68"/>
       <c r="H132" s="68"/>
       <c r="I132" s="68"/>
     </row>
-    <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A133" s="90" t="s">
-        <v>348</v>
-      </c>
-      <c r="B133" s="91" t="s">
+    <row r="133" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A133" s="91" t="s">
         <v>349</v>
       </c>
-      <c r="C133" s="68"/>
-      <c r="D133" s="68"/>
-      <c r="E133" s="68"/>
+      <c r="B133" s="92" t="s">
+        <v>350</v>
+      </c>
+      <c r="C133" s="18"/>
+      <c r="D133" s="8"/>
+      <c r="E133" s="74"/>
       <c r="F133" s="68"/>
       <c r="G133" s="68"/>
       <c r="H133" s="68"/>
       <c r="I133" s="68"/>
     </row>
-    <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A134" s="90" t="s">
-        <v>350</v>
-      </c>
-      <c r="B134" s="91" t="s">
+    <row r="134" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A134" s="93" t="s">
         <v>351</v>
+      </c>
+      <c r="B134" s="92" t="s">
+        <v>352</v>
       </c>
       <c r="C134" s="68"/>
       <c r="D134" s="68"/>
@@ -5496,11 +5530,11 @@
       <c r="I134" s="68"/>
     </row>
     <row r="135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A135" s="90" t="s">
-        <v>352</v>
-      </c>
-      <c r="B135" s="91" t="s">
+      <c r="A135" s="93" t="s">
         <v>353</v>
+      </c>
+      <c r="B135" s="92" t="s">
+        <v>354</v>
       </c>
       <c r="C135" s="68"/>
       <c r="D135" s="68"/>
@@ -5511,11 +5545,11 @@
       <c r="I135" s="68"/>
     </row>
     <row r="136" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A136" s="90" t="s">
-        <v>354</v>
-      </c>
-      <c r="B136" s="91" t="s">
+      <c r="A136" s="93" t="s">
         <v>355</v>
+      </c>
+      <c r="B136" s="92" t="s">
+        <v>356</v>
       </c>
       <c r="C136" s="68"/>
       <c r="D136" s="68"/>
@@ -5526,11 +5560,11 @@
       <c r="I136" s="68"/>
     </row>
     <row r="137" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A137" s="90" t="s">
-        <v>356</v>
-      </c>
-      <c r="B137" s="91" t="s">
+      <c r="A137" s="93" t="s">
         <v>357</v>
+      </c>
+      <c r="B137" s="92" t="s">
+        <v>358</v>
       </c>
       <c r="C137" s="68"/>
       <c r="D137" s="68"/>
@@ -5541,11 +5575,11 @@
       <c r="I137" s="68"/>
     </row>
     <row r="138" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A138" s="1" t="s">
-        <v>358</v>
-      </c>
-      <c r="B138" s="68" t="s">
+      <c r="A138" s="93" t="s">
         <v>359</v>
+      </c>
+      <c r="B138" s="92" t="s">
+        <v>360</v>
       </c>
       <c r="C138" s="68"/>
       <c r="D138" s="68"/>
@@ -5556,7 +5590,12 @@
       <c r="I138" s="68"/>
     </row>
     <row r="139" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B139" s="68"/>
+      <c r="A139" s="93" t="s">
+        <v>361</v>
+      </c>
+      <c r="B139" s="92" t="s">
+        <v>362</v>
+      </c>
       <c r="C139" s="68"/>
       <c r="D139" s="68"/>
       <c r="E139" s="68"/>
@@ -5576,7 +5615,6 @@
       <c r="I140" s="68"/>
     </row>
     <row r="141" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A141" s="68"/>
       <c r="B141" s="68"/>
       <c r="C141" s="68"/>
       <c r="D141" s="68"/>
@@ -5587,7 +5625,6 @@
       <c r="I141" s="68"/>
     </row>
     <row r="142" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A142" s="68"/>
       <c r="B142" s="68"/>
       <c r="C142" s="68"/>
       <c r="D142" s="68"/>
@@ -5597,11 +5634,9 @@
       <c r="H142" s="68"/>
       <c r="I142" s="68"/>
     </row>
-    <row r="143" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="143" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="68"/>
-      <c r="B143" s="92" t="s">
-        <v>360</v>
-      </c>
+      <c r="B143" s="68"/>
       <c r="C143" s="68"/>
       <c r="D143" s="68"/>
       <c r="E143" s="68"/>
@@ -5610,30 +5645,22 @@
       <c r="H143" s="68"/>
       <c r="I143" s="68"/>
     </row>
-    <row r="144" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A144" s="93"/>
-      <c r="B144" s="94" t="s">
-        <v>361</v>
-      </c>
-      <c r="C144" s="94" t="s">
-        <v>362</v>
-      </c>
-      <c r="D144" s="95" t="s">
-        <v>363</v>
-      </c>
-      <c r="E144" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F144" s="30" t="s">
-        <v>8</v>
-      </c>
+    <row r="144" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A144" s="68"/>
+      <c r="B144" s="68"/>
+      <c r="C144" s="68"/>
+      <c r="D144" s="68"/>
+      <c r="E144" s="68"/>
+      <c r="F144" s="68"/>
       <c r="G144" s="68"/>
       <c r="H144" s="68"/>
       <c r="I144" s="68"/>
     </row>
-    <row r="145" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A145" s="96"/>
-      <c r="B145" s="68"/>
+    <row r="145" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A145" s="68"/>
+      <c r="B145" s="94" t="s">
+        <v>363</v>
+      </c>
       <c r="C145" s="68"/>
       <c r="D145" s="68"/>
       <c r="E145" s="68"/>
@@ -5642,134 +5669,128 @@
       <c r="H145" s="68"/>
       <c r="I145" s="68"/>
     </row>
-    <row r="146" customFormat="false" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A146" s="97" t="s">
+    <row r="146" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A146" s="95"/>
+      <c r="B146" s="96" t="s">
         <v>364</v>
       </c>
-      <c r="B146" s="98" t="s">
+      <c r="C146" s="96" t="s">
         <v>365</v>
       </c>
-      <c r="C146" s="99" t="s">
+      <c r="D146" s="97" t="s">
         <v>366</v>
       </c>
-      <c r="D146" s="100" t="s">
-        <v>367</v>
-      </c>
-      <c r="E146" s="101" t="s">
-        <v>368</v>
-      </c>
-      <c r="F146" s="102" t="s">
-        <v>369</v>
+      <c r="E146" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F146" s="30" t="s">
+        <v>8</v>
       </c>
       <c r="G146" s="68"/>
       <c r="H146" s="68"/>
       <c r="I146" s="68"/>
     </row>
-    <row r="147" customFormat="false" ht="85.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A147" s="97"/>
-      <c r="B147" s="103" t="s">
-        <v>370</v>
-      </c>
-      <c r="C147" s="104" t="s">
-        <v>371</v>
-      </c>
-      <c r="D147" s="105" t="s">
-        <v>372</v>
-      </c>
-      <c r="E147" s="106" t="s">
-        <v>373</v>
-      </c>
-      <c r="F147" s="102" t="s">
-        <v>374</v>
-      </c>
+    <row r="147" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A147" s="98"/>
+      <c r="B147" s="68"/>
+      <c r="C147" s="68"/>
+      <c r="D147" s="68"/>
+      <c r="E147" s="68"/>
+      <c r="F147" s="68"/>
       <c r="G147" s="68"/>
       <c r="H147" s="68"/>
       <c r="I147" s="68"/>
     </row>
-    <row r="148" customFormat="false" ht="90.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A148" s="97"/>
-      <c r="B148" s="107" t="s">
-        <v>375</v>
-      </c>
-      <c r="C148" s="108" t="s">
-        <v>376</v>
-      </c>
-      <c r="D148" s="109" t="s">
-        <v>377</v>
-      </c>
-      <c r="E148" s="110" t="s">
-        <v>12</v>
-      </c>
-      <c r="F148" s="111" t="s">
-        <v>12</v>
-      </c>
-      <c r="G148" s="88" t="s">
-        <v>378</v>
-      </c>
+    <row r="148" customFormat="false" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A148" s="99" t="s">
+        <v>367</v>
+      </c>
+      <c r="B148" s="100" t="s">
+        <v>368</v>
+      </c>
+      <c r="C148" s="101" t="s">
+        <v>369</v>
+      </c>
+      <c r="D148" s="102" t="s">
+        <v>370</v>
+      </c>
+      <c r="E148" s="103" t="s">
+        <v>371</v>
+      </c>
+      <c r="F148" s="104" t="s">
+        <v>372</v>
+      </c>
+      <c r="G148" s="68"/>
       <c r="H148" s="68"/>
       <c r="I148" s="68"/>
-      <c r="J148" s="68"/>
-      <c r="K148" s="68"/>
-      <c r="L148" s="68"/>
-    </row>
-    <row r="149" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A149" s="97"/>
-      <c r="B149" s="112" t="s">
-        <v>379</v>
-      </c>
-      <c r="C149" s="108" t="s">
+    </row>
+    <row r="149" customFormat="false" ht="85.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A149" s="99"/>
+      <c r="B149" s="105" t="s">
+        <v>373</v>
+      </c>
+      <c r="C149" s="106" t="s">
+        <v>374</v>
+      </c>
+      <c r="D149" s="107" t="s">
+        <v>375</v>
+      </c>
+      <c r="E149" s="108" t="s">
         <v>376</v>
       </c>
-      <c r="D149" s="109" t="s">
-        <v>380</v>
-      </c>
-      <c r="E149" s="110" t="s">
-        <v>12</v>
-      </c>
-      <c r="F149" s="111" t="s">
-        <v>12</v>
-      </c>
-      <c r="G149" s="88" t="s">
-        <v>381</v>
-      </c>
+      <c r="F149" s="104" t="s">
+        <v>377</v>
+      </c>
+      <c r="G149" s="68"/>
       <c r="H149" s="68"/>
       <c r="I149" s="68"/>
-      <c r="J149" s="68"/>
-      <c r="K149" s="68"/>
-      <c r="L149" s="68"/>
-    </row>
-    <row r="150" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A150" s="97"/>
-      <c r="B150" s="113" t="s">
-        <v>382</v>
-      </c>
-      <c r="C150" s="114" t="s">
-        <v>376</v>
-      </c>
-      <c r="D150" s="115" t="s">
-        <v>383</v>
-      </c>
-      <c r="E150" s="116" t="s">
+    </row>
+    <row r="150" customFormat="false" ht="90.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A150" s="99"/>
+      <c r="B150" s="109" t="s">
+        <v>378</v>
+      </c>
+      <c r="C150" s="110" t="s">
+        <v>379</v>
+      </c>
+      <c r="D150" s="111" t="s">
+        <v>380</v>
+      </c>
+      <c r="E150" s="112" t="s">
         <v>12</v>
       </c>
-      <c r="F150" s="117" t="s">
+      <c r="F150" s="113" t="s">
         <v>12</v>
       </c>
-      <c r="G150" s="68"/>
+      <c r="G150" s="88" t="s">
+        <v>381</v>
+      </c>
       <c r="H150" s="68"/>
       <c r="I150" s="68"/>
       <c r="J150" s="68"/>
       <c r="K150" s="68"/>
       <c r="L150" s="68"/>
     </row>
-    <row r="151" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A151" s="68"/>
-      <c r="B151" s="68"/>
-      <c r="C151" s="68"/>
-      <c r="D151" s="68"/>
-      <c r="E151" s="68"/>
-      <c r="F151" s="68"/>
-      <c r="G151" s="68"/>
+    <row r="151" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A151" s="99"/>
+      <c r="B151" s="114" t="s">
+        <v>382</v>
+      </c>
+      <c r="C151" s="110" t="s">
+        <v>379</v>
+      </c>
+      <c r="D151" s="111" t="s">
+        <v>383</v>
+      </c>
+      <c r="E151" s="112" t="s">
+        <v>12</v>
+      </c>
+      <c r="F151" s="113" t="s">
+        <v>12</v>
+      </c>
+      <c r="G151" s="88" t="s">
+        <v>384</v>
+      </c>
       <c r="H151" s="68"/>
       <c r="I151" s="68"/>
       <c r="J151" s="68"/>
@@ -5777,12 +5798,22 @@
       <c r="L151" s="68"/>
     </row>
     <row r="152" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A152" s="68"/>
-      <c r="B152" s="68"/>
-      <c r="C152" s="68"/>
-      <c r="D152" s="68"/>
-      <c r="E152" s="68"/>
-      <c r="F152" s="68"/>
+      <c r="A152" s="99"/>
+      <c r="B152" s="115" t="s">
+        <v>385</v>
+      </c>
+      <c r="C152" s="116" t="s">
+        <v>379</v>
+      </c>
+      <c r="D152" s="117" t="s">
+        <v>386</v>
+      </c>
+      <c r="E152" s="118" t="s">
+        <v>12</v>
+      </c>
+      <c r="F152" s="119" t="s">
+        <v>12</v>
+      </c>
       <c r="G152" s="68"/>
       <c r="H152" s="68"/>
       <c r="I152" s="68"/>
@@ -5804,13 +5835,9 @@
       <c r="K153" s="68"/>
       <c r="L153" s="68"/>
     </row>
-    <row r="154" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A154" s="118" t="s">
-        <v>384</v>
-      </c>
-      <c r="B154" s="88" t="s">
-        <v>385</v>
-      </c>
+    <row r="154" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A154" s="68"/>
+      <c r="B154" s="68"/>
       <c r="C154" s="68"/>
       <c r="D154" s="68"/>
       <c r="E154" s="68"/>
@@ -5832,10 +5859,17 @@
       <c r="G155" s="68"/>
       <c r="H155" s="68"/>
       <c r="I155" s="68"/>
-    </row>
-    <row r="156" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A156" s="68"/>
-      <c r="B156" s="68"/>
+      <c r="J155" s="68"/>
+      <c r="K155" s="68"/>
+      <c r="L155" s="68"/>
+    </row>
+    <row r="156" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A156" s="120" t="s">
+        <v>387</v>
+      </c>
+      <c r="B156" s="88" t="s">
+        <v>388</v>
+      </c>
       <c r="C156" s="68"/>
       <c r="D156" s="68"/>
       <c r="E156" s="68"/>
@@ -5843,6 +5877,9 @@
       <c r="G156" s="68"/>
       <c r="H156" s="68"/>
       <c r="I156" s="68"/>
+      <c r="J156" s="68"/>
+      <c r="K156" s="68"/>
+      <c r="L156" s="68"/>
     </row>
     <row r="157" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="68"/>
@@ -7526,6 +7563,28 @@
       <c r="G309" s="68"/>
       <c r="H309" s="68"/>
       <c r="I309" s="68"/>
+    </row>
+    <row r="310" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A310" s="68"/>
+      <c r="B310" s="68"/>
+      <c r="C310" s="68"/>
+      <c r="D310" s="68"/>
+      <c r="E310" s="68"/>
+      <c r="F310" s="68"/>
+      <c r="G310" s="68"/>
+      <c r="H310" s="68"/>
+      <c r="I310" s="68"/>
+    </row>
+    <row r="311" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A311" s="68"/>
+      <c r="B311" s="68"/>
+      <c r="C311" s="68"/>
+      <c r="D311" s="68"/>
+      <c r="E311" s="68"/>
+      <c r="F311" s="68"/>
+      <c r="G311" s="68"/>
+      <c r="H311" s="68"/>
+      <c r="I311" s="68"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:J1"/>
@@ -7561,7 +7620,7 @@
     <mergeCell ref="F112:I112"/>
     <mergeCell ref="F114:J114"/>
     <mergeCell ref="F120:J120"/>
-    <mergeCell ref="A146:A150"/>
+    <mergeCell ref="A148:A152"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
remove sensors registers from hmi
</commit_message>
<xml_diff>
--- a/documentation/Tabla_de_registros_HMI_Ivan.xlsx
+++ b/documentation/Tabla_de_registros_HMI_Ivan.xlsx
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="705" uniqueCount="402">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="390">
   <si>
     <t xml:space="preserve">Elemento IOLink</t>
   </si>
@@ -1305,43 +1305,6 @@
   <si>
     <t xml:space="preserve">HEX --------DEC
 HR-0023 – HR-40035</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sensor_material_pressure </t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-HR-0024 – HR-40036</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sensor_material_temperature </t>
-  </si>
-  <si>
-    <t xml:space="preserve">HR-0025 – HR-40037</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sensor_laser_distance </t>
-  </si>
-  <si>
-    <t xml:space="preserve">HR-0026 -HR-40038</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sensor_pressure_regulator_read_set </t>
-  </si>
-  <si>
-    <t xml:space="preserve">HR-0027 – HR-40039</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sensor_pressure_regulator_read_real </t>
-  </si>
-  <si>
-    <t xml:space="preserve">HR-0028 – HR-40040</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sensor_pressure_regulator_valve_read_state </t>
-  </si>
-  <si>
-    <t xml:space="preserve">HR-0029 – HR-40041</t>
   </si>
   <si>
     <t xml:space="preserve">These are HMI registers</t>
@@ -1680,7 +1643,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="&quot; $&quot;* #,##0.00\ ;&quot;-$&quot;* #,##0.00\ ;&quot; $&quot;* \-#\ ;\ @\ "/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1751,7 +1714,14 @@
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF000000"/>
+      <color rgb="FFDEE6EF"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFDEE6EF"/>
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="1"/>
@@ -1855,7 +1825,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFDDE8CB"/>
-        <bgColor rgb="FFFFF5CE"/>
+        <bgColor rgb="FFDEE6EF"/>
       </patternFill>
     </fill>
     <fill>
@@ -2169,7 +2139,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="130">
+  <cellXfs count="131">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2554,11 +2524,15 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2662,31 +2636,31 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="17" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2722,7 +2696,7 @@
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FFFFFFD7"/>
-      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFDEE6EF"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
@@ -2806,7 +2780,7 @@
   <dimension ref="A1:L311"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A117" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A96" activeCellId="0" sqref="A96"/>
+      <selection pane="topLeft" activeCell="B142" activeCellId="0" sqref="B142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5835,13 +5809,9 @@
       <c r="H133" s="71"/>
       <c r="I133" s="71"/>
     </row>
-    <row r="134" customFormat="false" ht="27.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A134" s="96" t="s">
-        <v>352</v>
-      </c>
-      <c r="B134" s="95" t="s">
-        <v>353</v>
-      </c>
+    <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A134" s="96"/>
+      <c r="B134" s="97"/>
       <c r="C134" s="71"/>
       <c r="D134" s="71"/>
       <c r="E134" s="71"/>
@@ -5851,12 +5821,8 @@
       <c r="I134" s="71"/>
     </row>
     <row r="135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A135" s="96" t="s">
-        <v>354</v>
-      </c>
-      <c r="B135" s="95" t="s">
-        <v>355</v>
-      </c>
+      <c r="A135" s="96"/>
+      <c r="B135" s="97"/>
       <c r="C135" s="71"/>
       <c r="D135" s="71"/>
       <c r="E135" s="71"/>
@@ -5866,12 +5832,8 @@
       <c r="I135" s="71"/>
     </row>
     <row r="136" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A136" s="96" t="s">
-        <v>356</v>
-      </c>
-      <c r="B136" s="95" t="s">
-        <v>357</v>
-      </c>
+      <c r="A136" s="96"/>
+      <c r="B136" s="97"/>
       <c r="C136" s="71"/>
       <c r="D136" s="71"/>
       <c r="E136" s="71"/>
@@ -5881,12 +5843,8 @@
       <c r="I136" s="71"/>
     </row>
     <row r="137" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A137" s="96" t="s">
-        <v>358</v>
-      </c>
-      <c r="B137" s="95" t="s">
-        <v>359</v>
-      </c>
+      <c r="A137" s="96"/>
+      <c r="B137" s="97"/>
       <c r="C137" s="71"/>
       <c r="D137" s="71"/>
       <c r="E137" s="71"/>
@@ -5896,12 +5854,8 @@
       <c r="I137" s="71"/>
     </row>
     <row r="138" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A138" s="96" t="s">
-        <v>360</v>
-      </c>
-      <c r="B138" s="95" t="s">
-        <v>361</v>
-      </c>
+      <c r="A138" s="96"/>
+      <c r="B138" s="97"/>
       <c r="C138" s="71"/>
       <c r="D138" s="71"/>
       <c r="E138" s="71"/>
@@ -5911,12 +5865,8 @@
       <c r="I138" s="71"/>
     </row>
     <row r="139" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A139" s="96" t="s">
-        <v>362</v>
-      </c>
-      <c r="B139" s="95" t="s">
-        <v>363</v>
-      </c>
+      <c r="A139" s="96"/>
+      <c r="B139" s="97"/>
       <c r="C139" s="71"/>
       <c r="D139" s="71"/>
       <c r="E139" s="71"/>
@@ -5979,8 +5929,8 @@
     </row>
     <row r="145" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="71"/>
-      <c r="B145" s="97" t="s">
-        <v>364</v>
+      <c r="B145" s="98" t="s">
+        <v>352</v>
       </c>
       <c r="C145" s="71"/>
       <c r="D145" s="71"/>
@@ -5991,15 +5941,15 @@
       <c r="I145" s="71"/>
     </row>
     <row r="146" customFormat="false" ht="27.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A146" s="98"/>
-      <c r="B146" s="99" t="s">
-        <v>365</v>
-      </c>
-      <c r="C146" s="99" t="s">
-        <v>366</v>
-      </c>
-      <c r="D146" s="100" t="s">
-        <v>367</v>
+      <c r="A146" s="99"/>
+      <c r="B146" s="100" t="s">
+        <v>353</v>
+      </c>
+      <c r="C146" s="100" t="s">
+        <v>354</v>
+      </c>
+      <c r="D146" s="101" t="s">
+        <v>355</v>
       </c>
       <c r="E146" s="9" t="s">
         <v>7</v>
@@ -6012,7 +5962,7 @@
       <c r="I146" s="71"/>
     </row>
     <row r="147" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A147" s="101"/>
+      <c r="A147" s="102"/>
       <c r="B147" s="71"/>
       <c r="C147" s="71"/>
       <c r="D147" s="71"/>
@@ -6023,68 +5973,68 @@
       <c r="I147" s="71"/>
     </row>
     <row r="148" customFormat="false" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A148" s="102" t="s">
-        <v>368</v>
-      </c>
-      <c r="B148" s="103" t="s">
-        <v>369</v>
-      </c>
-      <c r="C148" s="104" t="s">
-        <v>370</v>
-      </c>
-      <c r="D148" s="105" t="s">
-        <v>371</v>
-      </c>
-      <c r="E148" s="106" t="s">
-        <v>372</v>
-      </c>
-      <c r="F148" s="107" t="s">
-        <v>373</v>
+      <c r="A148" s="103" t="s">
+        <v>356</v>
+      </c>
+      <c r="B148" s="104" t="s">
+        <v>357</v>
+      </c>
+      <c r="C148" s="105" t="s">
+        <v>358</v>
+      </c>
+      <c r="D148" s="106" t="s">
+        <v>359</v>
+      </c>
+      <c r="E148" s="107" t="s">
+        <v>360</v>
+      </c>
+      <c r="F148" s="108" t="s">
+        <v>361</v>
       </c>
       <c r="G148" s="71"/>
       <c r="H148" s="71"/>
       <c r="I148" s="71"/>
     </row>
     <row r="149" customFormat="false" ht="85.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A149" s="102"/>
-      <c r="B149" s="108" t="s">
-        <v>374</v>
-      </c>
-      <c r="C149" s="109" t="s">
-        <v>375</v>
-      </c>
-      <c r="D149" s="110" t="s">
-        <v>376</v>
-      </c>
-      <c r="E149" s="111" t="s">
-        <v>377</v>
-      </c>
-      <c r="F149" s="107" t="s">
-        <v>378</v>
+      <c r="A149" s="103"/>
+      <c r="B149" s="109" t="s">
+        <v>362</v>
+      </c>
+      <c r="C149" s="110" t="s">
+        <v>363</v>
+      </c>
+      <c r="D149" s="111" t="s">
+        <v>364</v>
+      </c>
+      <c r="E149" s="112" t="s">
+        <v>365</v>
+      </c>
+      <c r="F149" s="108" t="s">
+        <v>366</v>
       </c>
       <c r="G149" s="71"/>
       <c r="H149" s="71"/>
       <c r="I149" s="71"/>
     </row>
     <row r="150" customFormat="false" ht="93.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A150" s="102"/>
-      <c r="B150" s="112" t="s">
-        <v>379</v>
-      </c>
-      <c r="C150" s="113" t="s">
-        <v>380</v>
-      </c>
-      <c r="D150" s="114" t="s">
-        <v>381</v>
-      </c>
-      <c r="E150" s="115" t="s">
+      <c r="A150" s="103"/>
+      <c r="B150" s="113" t="s">
+        <v>367</v>
+      </c>
+      <c r="C150" s="114" t="s">
+        <v>368</v>
+      </c>
+      <c r="D150" s="115" t="s">
+        <v>369</v>
+      </c>
+      <c r="E150" s="116" t="s">
         <v>12</v>
       </c>
-      <c r="F150" s="116" t="s">
+      <c r="F150" s="117" t="s">
         <v>12</v>
       </c>
       <c r="G150" s="91" t="s">
-        <v>382</v>
+        <v>370</v>
       </c>
       <c r="H150" s="71"/>
       <c r="I150" s="71"/>
@@ -6093,24 +6043,24 @@
       <c r="L150" s="71"/>
     </row>
     <row r="151" customFormat="false" ht="54.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A151" s="102"/>
-      <c r="B151" s="117" t="s">
-        <v>383</v>
-      </c>
-      <c r="C151" s="113" t="s">
-        <v>380</v>
-      </c>
-      <c r="D151" s="114" t="s">
-        <v>384</v>
-      </c>
-      <c r="E151" s="115" t="s">
+      <c r="A151" s="103"/>
+      <c r="B151" s="118" t="s">
+        <v>371</v>
+      </c>
+      <c r="C151" s="114" t="s">
+        <v>368</v>
+      </c>
+      <c r="D151" s="115" t="s">
+        <v>372</v>
+      </c>
+      <c r="E151" s="116" t="s">
         <v>12</v>
       </c>
-      <c r="F151" s="116" t="s">
+      <c r="F151" s="117" t="s">
         <v>12</v>
       </c>
       <c r="G151" s="91" t="s">
-        <v>385</v>
+        <v>373</v>
       </c>
       <c r="H151" s="71"/>
       <c r="I151" s="71"/>
@@ -6119,20 +6069,20 @@
       <c r="L151" s="71"/>
     </row>
     <row r="152" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A152" s="102"/>
-      <c r="B152" s="118" t="s">
-        <v>386</v>
-      </c>
-      <c r="C152" s="119" t="s">
-        <v>380</v>
-      </c>
-      <c r="D152" s="120" t="s">
-        <v>387</v>
-      </c>
-      <c r="E152" s="121" t="s">
+      <c r="A152" s="103"/>
+      <c r="B152" s="119" t="s">
+        <v>374</v>
+      </c>
+      <c r="C152" s="120" t="s">
+        <v>368</v>
+      </c>
+      <c r="D152" s="121" t="s">
+        <v>375</v>
+      </c>
+      <c r="E152" s="122" t="s">
         <v>12</v>
       </c>
-      <c r="F152" s="122" t="s">
+      <c r="F152" s="123" t="s">
         <v>12</v>
       </c>
       <c r="G152" s="71"/>
@@ -6185,11 +6135,11 @@
       <c r="L155" s="71"/>
     </row>
     <row r="156" customFormat="false" ht="54.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A156" s="123" t="s">
-        <v>388</v>
+      <c r="A156" s="124" t="s">
+        <v>376</v>
       </c>
       <c r="B156" s="91" t="s">
-        <v>389</v>
+        <v>377</v>
       </c>
       <c r="C156" s="71"/>
       <c r="D156" s="71"/>
@@ -7968,60 +7918,60 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="17.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="124" width="75.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="124" width="43.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="124" width="47.92"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="4" style="124" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="125" width="75.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="125" width="43.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="125" width="47.92"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="4" style="125" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="125" t="s">
-        <v>390</v>
-      </c>
-      <c r="B1" s="125" t="s">
-        <v>391</v>
-      </c>
-      <c r="C1" s="125" t="s">
-        <v>392</v>
+      <c r="A1" s="126" t="s">
+        <v>378</v>
+      </c>
+      <c r="B1" s="126" t="s">
+        <v>379</v>
+      </c>
+      <c r="C1" s="126" t="s">
+        <v>380</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="71.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="126" t="s">
-        <v>393</v>
-      </c>
-      <c r="B2" s="124" t="s">
-        <v>394</v>
+      <c r="A2" s="127" t="s">
+        <v>381</v>
+      </c>
+      <c r="B2" s="125" t="s">
+        <v>382</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="71.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="126" t="s">
-        <v>395</v>
+      <c r="A3" s="127" t="s">
+        <v>383</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="239.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="127" t="s">
-        <v>396</v>
+      <c r="A4" s="128" t="s">
+        <v>384</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="128" t="s">
-        <v>397</v>
-      </c>
-      <c r="B5" s="124" t="s">
-        <v>398</v>
+      <c r="A5" s="129" t="s">
+        <v>385</v>
+      </c>
+      <c r="B5" s="125" t="s">
+        <v>386</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="134.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="129" t="s">
-        <v>399</v>
+      <c r="A6" s="130" t="s">
+        <v>387</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="107.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="126" t="s">
-        <v>400</v>
-      </c>
-      <c r="B7" s="124" t="s">
-        <v>401</v>
+      <c r="A7" s="127" t="s">
+        <v>388</v>
+      </c>
+      <c r="B7" s="125" t="s">
+        <v>389</v>
       </c>
     </row>
   </sheetData>

</xml_diff>